<commit_message>
Q2 2022 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-18REOD_2018PSNA_Qrt.xlsx
+++ b/Data/National Accounts/PSA-18REOD_2018PSNA_Qrt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\Desktop\PSA\NAP\NAP\Q1 2022\Qtr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of August 2022\Qtr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BE8592-5B07-4168-BBD6-B47D08B5CCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E3D229-FF97-4AAE-9393-BACD97532A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REOD" sheetId="12" r:id="rId1"/>
@@ -324,7 +324,7 @@
     <definedName name="pet">#REF!</definedName>
     <definedName name="plastic">#REF!</definedName>
     <definedName name="ply">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">REOD!$A$1:$CN$132</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">REOD!$A$1:$CM$132</definedName>
     <definedName name="_xlnm.Print_Area">#REF!</definedName>
     <definedName name="PRINT_AREA_MI">#REF!</definedName>
     <definedName name="Print_Titles_MI">'[10]CAP93+'!$A$1:$IV$1,'[10]CAP93+'!$A$1:$A$65536</definedName>
@@ -469,7 +469,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="51">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -615,13 +615,13 @@
     <t>2021 - 2022</t>
   </si>
   <si>
-    <t>As of May 2022</t>
+    <t>As of August 2022</t>
   </si>
   <si>
-    <t>Q1 2000 to Q1 2022</t>
+    <t>Q1 2000 to Q2 2022</t>
   </si>
   <si>
-    <t>Q1 2001 to Q1 2022</t>
+    <t>Q1 2001 to Q2 2022</t>
   </si>
 </sst>
 </file>
@@ -629,10 +629,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -703,12 +703,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -729,56 +731,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2 2" xfId="4" xr:uid="{216CD568-AC7C-4D0D-9201-E09706422380}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{679523F5-E8A6-450A-BB7D-B9830CFC0309}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -23632,191 +23614,189 @@
   </sheetPr>
   <dimension ref="A1:EU132"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A52" colorId="22" zoomScale="62" zoomScaleNormal="62" zoomScaleSheetLayoutView="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BM1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="62" zoomScaleNormal="62" zoomScaleSheetLayoutView="62" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CC1" activePane="topRight" state="frozen"/>
       <selection activeCell="N19" sqref="N19"/>
-      <selection pane="topRight" activeCell="CI64" sqref="CI64:CN80"/>
+      <selection pane="topRight" activeCell="CH1" sqref="CH1:CM1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="3" customWidth="1"/>
-    <col min="2" max="73" width="8.33203125" style="3" customWidth="1"/>
-    <col min="74" max="77" width="8.33203125" style="17" customWidth="1"/>
-    <col min="78" max="78" width="9.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="79" max="90" width="8.33203125" style="3" customWidth="1"/>
-    <col min="91" max="16384" width="7.77734375" style="3"/>
+    <col min="1" max="1" width="38.36328125" style="3" customWidth="1"/>
+    <col min="2" max="91" width="8.36328125" style="3" customWidth="1"/>
+    <col min="92" max="16384" width="7.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="26">
+      <c r="B9" s="22">
         <v>2000</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22">
         <v>2001</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26">
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22">
         <v>2002</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26">
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
         <v>2003</v>
       </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26">
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22">
         <v>2004</v>
       </c>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="26">
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22">
         <v>2005</v>
       </c>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26">
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22">
         <v>2006</v>
       </c>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26">
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22">
         <v>2007</v>
       </c>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
-      <c r="AH9" s="26">
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="22">
         <v>2008</v>
       </c>
-      <c r="AI9" s="26"/>
-      <c r="AJ9" s="26"/>
-      <c r="AK9" s="26"/>
-      <c r="AL9" s="26">
+      <c r="AI9" s="22"/>
+      <c r="AJ9" s="22"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22">
         <v>2009</v>
       </c>
-      <c r="AM9" s="26"/>
-      <c r="AN9" s="26"/>
-      <c r="AO9" s="26"/>
-      <c r="AP9" s="26">
+      <c r="AM9" s="22"/>
+      <c r="AN9" s="22"/>
+      <c r="AO9" s="22"/>
+      <c r="AP9" s="22">
         <v>2010</v>
       </c>
-      <c r="AQ9" s="26"/>
-      <c r="AR9" s="26"/>
-      <c r="AS9" s="26"/>
-      <c r="AT9" s="26">
+      <c r="AQ9" s="22"/>
+      <c r="AR9" s="22"/>
+      <c r="AS9" s="22"/>
+      <c r="AT9" s="22">
         <v>2011</v>
       </c>
-      <c r="AU9" s="26"/>
-      <c r="AV9" s="26"/>
-      <c r="AW9" s="26"/>
-      <c r="AX9" s="26">
+      <c r="AU9" s="22"/>
+      <c r="AV9" s="22"/>
+      <c r="AW9" s="22"/>
+      <c r="AX9" s="22">
         <v>2012</v>
       </c>
-      <c r="AY9" s="26"/>
-      <c r="AZ9" s="26"/>
-      <c r="BA9" s="26"/>
-      <c r="BB9" s="26">
+      <c r="AY9" s="22"/>
+      <c r="AZ9" s="22"/>
+      <c r="BA9" s="22"/>
+      <c r="BB9" s="22">
         <v>2013</v>
       </c>
-      <c r="BC9" s="26"/>
-      <c r="BD9" s="26"/>
-      <c r="BE9" s="26"/>
-      <c r="BF9" s="26">
+      <c r="BC9" s="22"/>
+      <c r="BD9" s="22"/>
+      <c r="BE9" s="22"/>
+      <c r="BF9" s="22">
         <v>2014</v>
       </c>
-      <c r="BG9" s="26"/>
-      <c r="BH9" s="26"/>
-      <c r="BI9" s="26"/>
-      <c r="BJ9" s="26">
+      <c r="BG9" s="22"/>
+      <c r="BH9" s="22"/>
+      <c r="BI9" s="22"/>
+      <c r="BJ9" s="22">
         <v>2015</v>
       </c>
-      <c r="BK9" s="26"/>
-      <c r="BL9" s="26"/>
-      <c r="BM9" s="26"/>
-      <c r="BN9" s="26">
+      <c r="BK9" s="22"/>
+      <c r="BL9" s="22"/>
+      <c r="BM9" s="22"/>
+      <c r="BN9" s="22">
         <v>2016</v>
       </c>
-      <c r="BO9" s="26"/>
-      <c r="BP9" s="26"/>
-      <c r="BQ9" s="26"/>
-      <c r="BR9" s="26">
+      <c r="BO9" s="22"/>
+      <c r="BP9" s="22"/>
+      <c r="BQ9" s="22"/>
+      <c r="BR9" s="22">
         <v>2017</v>
       </c>
-      <c r="BS9" s="26"/>
-      <c r="BT9" s="26"/>
-      <c r="BU9" s="26"/>
-      <c r="BV9" s="29">
+      <c r="BS9" s="22"/>
+      <c r="BT9" s="22"/>
+      <c r="BU9" s="22"/>
+      <c r="BV9" s="22">
         <v>2018</v>
       </c>
-      <c r="BW9" s="29"/>
-      <c r="BX9" s="29"/>
-      <c r="BY9" s="29"/>
-      <c r="BZ9" s="26">
+      <c r="BW9" s="22"/>
+      <c r="BX9" s="22"/>
+      <c r="BY9" s="22"/>
+      <c r="BZ9" s="22">
         <v>2019</v>
       </c>
-      <c r="CA9" s="26"/>
-      <c r="CB9" s="26"/>
-      <c r="CC9" s="26"/>
-      <c r="CD9" s="26">
+      <c r="CA9" s="22"/>
+      <c r="CB9" s="22"/>
+      <c r="CC9" s="22"/>
+      <c r="CD9" s="22">
         <v>2020</v>
       </c>
-      <c r="CE9" s="26"/>
-      <c r="CF9" s="26"/>
-      <c r="CG9" s="26"/>
-      <c r="CH9" s="26">
+      <c r="CE9" s="22"/>
+      <c r="CF9" s="22"/>
+      <c r="CG9" s="22"/>
+      <c r="CH9" s="22">
         <v>2021</v>
       </c>
-      <c r="CI9" s="26"/>
-      <c r="CJ9" s="26"/>
-      <c r="CK9" s="26"/>
-      <c r="CL9" s="25">
+      <c r="CI9" s="22"/>
+      <c r="CJ9" s="22"/>
+      <c r="CK9" s="22"/>
+      <c r="CL9" s="22">
         <v>2022</v>
       </c>
+      <c r="CM9" s="22"/>
     </row>
-    <row r="10" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -24036,16 +24016,16 @@
       <c r="BU10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="BV10" s="18" t="s">
+      <c r="BV10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="BW10" s="18" t="s">
+      <c r="BW10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="BX10" s="18" t="s">
+      <c r="BX10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="BY10" s="18" t="s">
+      <c r="BY10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="BZ10" s="6" t="s">
@@ -24087,11 +24067,14 @@
       <c r="CL10" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="CM10" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -24311,40 +24294,40 @@
       <c r="BU12" s="15">
         <v>145861.00348794594</v>
       </c>
-      <c r="BV12" s="19">
+      <c r="BV12" s="17">
         <v>146854.24472862401</v>
       </c>
-      <c r="BW12" s="19">
+      <c r="BW12" s="17">
         <v>166776.45018528201</v>
       </c>
-      <c r="BX12" s="19">
+      <c r="BX12" s="17">
         <v>176507.61409786201</v>
       </c>
-      <c r="BY12" s="19">
+      <c r="BY12" s="17">
         <v>161269.1348491307</v>
       </c>
-      <c r="BZ12" s="15">
+      <c r="BZ12" s="17">
         <v>161070.66317850101</v>
       </c>
-      <c r="CA12" s="15">
+      <c r="CA12" s="17">
         <v>178363.90625445903</v>
       </c>
-      <c r="CB12" s="15">
+      <c r="CB12" s="17">
         <v>189093.06232804793</v>
       </c>
-      <c r="CC12" s="15">
+      <c r="CC12" s="17">
         <v>163483.19961062953</v>
       </c>
-      <c r="CD12" s="15">
+      <c r="CD12" s="17">
         <v>154557.66416923361</v>
       </c>
-      <c r="CE12" s="15">
+      <c r="CE12" s="17">
         <v>83141.367183577007</v>
       </c>
-      <c r="CF12" s="15">
+      <c r="CF12" s="17">
         <v>128379.64827916201</v>
       </c>
-      <c r="CG12" s="15">
+      <c r="CG12" s="17">
         <v>124488.42840152988</v>
       </c>
       <c r="CH12" s="15">
@@ -24360,9 +24343,11 @@
         <v>138425.43993440329</v>
       </c>
       <c r="CL12" s="15">
-        <v>149378.87372352509</v>
-      </c>
-      <c r="CM12" s="11"/>
+        <v>143436.29439306865</v>
+      </c>
+      <c r="CM12" s="15">
+        <v>141905.18180495873</v>
+      </c>
       <c r="CN12" s="11"/>
       <c r="CO12" s="11"/>
       <c r="CP12" s="11"/>
@@ -24424,7 +24409,7 @@
       <c r="ET12" s="11"/>
       <c r="EU12" s="11"/>
     </row>
-    <row r="13" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -24644,40 +24629,40 @@
       <c r="BU13" s="15">
         <v>126199.64162271524</v>
       </c>
-      <c r="BV13" s="19">
+      <c r="BV13" s="17">
         <v>131656.53034154201</v>
       </c>
-      <c r="BW13" s="19">
+      <c r="BW13" s="17">
         <v>134817.764547178</v>
       </c>
-      <c r="BX13" s="19">
+      <c r="BX13" s="17">
         <v>137126.375535139</v>
       </c>
-      <c r="BY13" s="19">
+      <c r="BY13" s="17">
         <v>134664.53180269324</v>
       </c>
-      <c r="BZ13" s="15">
+      <c r="BZ13" s="17">
         <v>138368.06774773693</v>
       </c>
-      <c r="CA13" s="15">
+      <c r="CA13" s="17">
         <v>140973.88666726652</v>
       </c>
-      <c r="CB13" s="15">
+      <c r="CB13" s="17">
         <v>143789.87396310209</v>
       </c>
-      <c r="CC13" s="15">
+      <c r="CC13" s="17">
         <v>140500.95675457982</v>
       </c>
-      <c r="CD13" s="15">
+      <c r="CD13" s="17">
         <v>145927.77943950184</v>
       </c>
-      <c r="CE13" s="15">
+      <c r="CE13" s="17">
         <v>148418.65486251179</v>
       </c>
-      <c r="CF13" s="15">
+      <c r="CF13" s="17">
         <v>150354.47324956354</v>
       </c>
-      <c r="CG13" s="15">
+      <c r="CG13" s="17">
         <v>146344.17741600078</v>
       </c>
       <c r="CH13" s="15">
@@ -24695,7 +24680,9 @@
       <c r="CL13" s="15">
         <v>154044.26758366541</v>
       </c>
-      <c r="CM13" s="11"/>
+      <c r="CM13" s="15">
+        <v>156305.18516723299</v>
+      </c>
       <c r="CN13" s="11"/>
       <c r="CO13" s="11"/>
       <c r="CP13" s="11"/>
@@ -24757,7 +24744,7 @@
       <c r="ET13" s="11"/>
       <c r="EU13" s="11"/>
     </row>
-    <row r="14" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -24830,10 +24817,10 @@
       <c r="BS14" s="11"/>
       <c r="BT14" s="11"/>
       <c r="BU14" s="11"/>
-      <c r="BV14" s="20"/>
-      <c r="BW14" s="20"/>
-      <c r="BX14" s="20"/>
-      <c r="BY14" s="20"/>
+      <c r="BV14" s="11"/>
+      <c r="BW14" s="11"/>
+      <c r="BX14" s="11"/>
+      <c r="BY14" s="11"/>
       <c r="BZ14" s="11"/>
       <c r="CA14" s="11"/>
       <c r="CB14" s="11"/>
@@ -24909,7 +24896,7 @@
       <c r="ET14" s="11"/>
       <c r="EU14" s="11"/>
     </row>
-    <row r="15" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -25129,40 +25116,40 @@
       <c r="BU15" s="16">
         <v>272060.64511066116</v>
       </c>
-      <c r="BV15" s="21">
+      <c r="BV15" s="18">
         <v>278510.77507016598</v>
       </c>
-      <c r="BW15" s="21">
+      <c r="BW15" s="18">
         <v>301594.21473245998</v>
       </c>
-      <c r="BX15" s="21">
+      <c r="BX15" s="18">
         <v>313633.98963300104</v>
       </c>
-      <c r="BY15" s="21">
+      <c r="BY15" s="18">
         <v>295933.66665182391</v>
       </c>
-      <c r="BZ15" s="16">
+      <c r="BZ15" s="18">
         <v>299438.73092623794</v>
       </c>
-      <c r="CA15" s="16">
+      <c r="CA15" s="18">
         <v>319337.79292172554</v>
       </c>
-      <c r="CB15" s="16">
+      <c r="CB15" s="18">
         <v>332882.93629115005</v>
       </c>
-      <c r="CC15" s="16">
+      <c r="CC15" s="18">
         <v>303984.15636520938</v>
       </c>
-      <c r="CD15" s="16">
+      <c r="CD15" s="18">
         <v>300485.44360873546</v>
       </c>
-      <c r="CE15" s="16">
+      <c r="CE15" s="18">
         <v>231560.02204608879</v>
       </c>
-      <c r="CF15" s="16">
+      <c r="CF15" s="18">
         <v>278734.12152872555</v>
       </c>
-      <c r="CG15" s="16">
+      <c r="CG15" s="18">
         <v>270832.60581753065</v>
       </c>
       <c r="CH15" s="16">
@@ -25178,9 +25165,11 @@
         <v>288031.46561385342</v>
       </c>
       <c r="CL15" s="16">
-        <v>303423.14130719053</v>
-      </c>
-      <c r="CM15" s="11"/>
+        <v>297480.56197673408</v>
+      </c>
+      <c r="CM15" s="16">
+        <v>298210.36697219172</v>
+      </c>
       <c r="CN15" s="11"/>
       <c r="CO15" s="11"/>
       <c r="CP15" s="11"/>
@@ -25242,7 +25231,7 @@
       <c r="ET15" s="11"/>
       <c r="EU15" s="11"/>
     </row>
-    <row r="16" spans="1:151" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:151" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -25316,10 +25305,10 @@
       <c r="BS16" s="9"/>
       <c r="BT16" s="9"/>
       <c r="BU16" s="9"/>
-      <c r="BV16" s="22"/>
-      <c r="BW16" s="22"/>
-      <c r="BX16" s="22"/>
-      <c r="BY16" s="22"/>
+      <c r="BV16" s="9"/>
+      <c r="BW16" s="9"/>
+      <c r="BX16" s="9"/>
+      <c r="BY16" s="9"/>
       <c r="BZ16" s="9"/>
       <c r="CA16" s="9"/>
       <c r="CB16" s="9"/>
@@ -25333,13 +25322,14 @@
       <c r="CJ16" s="9"/>
       <c r="CK16" s="9"/>
       <c r="CL16" s="9"/>
+      <c r="CM16" s="9"/>
     </row>
-    <row r="17" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -25412,10 +25402,10 @@
       <c r="BS18" s="11"/>
       <c r="BT18" s="11"/>
       <c r="BU18" s="11"/>
-      <c r="BV18" s="20"/>
-      <c r="BW18" s="20"/>
-      <c r="BX18" s="20"/>
-      <c r="BY18" s="20"/>
+      <c r="BV18" s="11"/>
+      <c r="BW18" s="11"/>
+      <c r="BX18" s="11"/>
+      <c r="BY18" s="11"/>
       <c r="BZ18" s="11"/>
       <c r="CA18" s="11"/>
       <c r="CB18" s="11"/>
@@ -25491,7 +25481,7 @@
       <c r="ET18" s="11"/>
       <c r="EU18" s="11"/>
     </row>
-    <row r="19" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -25564,10 +25554,10 @@
       <c r="BS19" s="11"/>
       <c r="BT19" s="11"/>
       <c r="BU19" s="11"/>
-      <c r="BV19" s="20"/>
-      <c r="BW19" s="20"/>
-      <c r="BX19" s="20"/>
-      <c r="BY19" s="20"/>
+      <c r="BV19" s="11"/>
+      <c r="BW19" s="11"/>
+      <c r="BX19" s="11"/>
+      <c r="BY19" s="11"/>
       <c r="BZ19" s="11"/>
       <c r="CA19" s="11"/>
       <c r="CB19" s="11"/>
@@ -25643,175 +25633,176 @@
       <c r="ET19" s="11"/>
       <c r="EU19" s="11"/>
     </row>
-    <row r="20" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="26">
+      <c r="B28" s="22">
         <v>2000</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="26">
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="22">
         <v>2001</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="26">
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="22">
         <v>2002</v>
       </c>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="26">
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="22">
         <v>2003</v>
       </c>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="26">
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="22">
         <v>2004</v>
       </c>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="26">
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="22">
         <v>2005</v>
       </c>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
-      <c r="Y28" s="27"/>
-      <c r="Z28" s="26">
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="Z28" s="22">
         <v>2006</v>
       </c>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="27"/>
-      <c r="AC28" s="27"/>
-      <c r="AD28" s="26">
+      <c r="AA28" s="24"/>
+      <c r="AB28" s="24"/>
+      <c r="AC28" s="24"/>
+      <c r="AD28" s="22">
         <v>2007</v>
       </c>
-      <c r="AE28" s="27"/>
-      <c r="AF28" s="27"/>
-      <c r="AG28" s="27"/>
-      <c r="AH28" s="26">
+      <c r="AE28" s="24"/>
+      <c r="AF28" s="24"/>
+      <c r="AG28" s="24"/>
+      <c r="AH28" s="22">
         <v>2008</v>
       </c>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="27"/>
-      <c r="AK28" s="27"/>
-      <c r="AL28" s="26">
+      <c r="AI28" s="24"/>
+      <c r="AJ28" s="24"/>
+      <c r="AK28" s="24"/>
+      <c r="AL28" s="22">
         <v>2009</v>
       </c>
-      <c r="AM28" s="27"/>
-      <c r="AN28" s="27"/>
-      <c r="AO28" s="27"/>
-      <c r="AP28" s="26">
+      <c r="AM28" s="24"/>
+      <c r="AN28" s="24"/>
+      <c r="AO28" s="24"/>
+      <c r="AP28" s="22">
         <v>2010</v>
       </c>
-      <c r="AQ28" s="27"/>
-      <c r="AR28" s="27"/>
-      <c r="AS28" s="27"/>
-      <c r="AT28" s="26">
+      <c r="AQ28" s="24"/>
+      <c r="AR28" s="24"/>
+      <c r="AS28" s="24"/>
+      <c r="AT28" s="22">
         <v>2011</v>
       </c>
-      <c r="AU28" s="27"/>
-      <c r="AV28" s="27"/>
-      <c r="AW28" s="27"/>
-      <c r="AX28" s="26">
+      <c r="AU28" s="24"/>
+      <c r="AV28" s="24"/>
+      <c r="AW28" s="24"/>
+      <c r="AX28" s="22">
         <v>2012</v>
       </c>
-      <c r="AY28" s="27"/>
-      <c r="AZ28" s="27"/>
-      <c r="BA28" s="27"/>
-      <c r="BB28" s="26">
+      <c r="AY28" s="24"/>
+      <c r="AZ28" s="24"/>
+      <c r="BA28" s="24"/>
+      <c r="BB28" s="22">
         <v>2013</v>
       </c>
-      <c r="BC28" s="27"/>
-      <c r="BD28" s="27"/>
-      <c r="BE28" s="27"/>
-      <c r="BF28" s="26">
+      <c r="BC28" s="24"/>
+      <c r="BD28" s="24"/>
+      <c r="BE28" s="24"/>
+      <c r="BF28" s="22">
         <v>2014</v>
       </c>
-      <c r="BG28" s="27"/>
-      <c r="BH28" s="27"/>
-      <c r="BI28" s="27"/>
-      <c r="BJ28" s="26">
+      <c r="BG28" s="24"/>
+      <c r="BH28" s="24"/>
+      <c r="BI28" s="24"/>
+      <c r="BJ28" s="22">
         <v>2015</v>
       </c>
-      <c r="BK28" s="27"/>
-      <c r="BL28" s="27"/>
-      <c r="BM28" s="27"/>
-      <c r="BN28" s="26">
+      <c r="BK28" s="24"/>
+      <c r="BL28" s="24"/>
+      <c r="BM28" s="24"/>
+      <c r="BN28" s="22">
         <v>2016</v>
       </c>
-      <c r="BO28" s="27"/>
-      <c r="BP28" s="27"/>
-      <c r="BQ28" s="27"/>
-      <c r="BR28" s="26">
+      <c r="BO28" s="24"/>
+      <c r="BP28" s="24"/>
+      <c r="BQ28" s="24"/>
+      <c r="BR28" s="22">
         <v>2017</v>
       </c>
-      <c r="BS28" s="27"/>
-      <c r="BT28" s="27"/>
-      <c r="BU28" s="27"/>
-      <c r="BV28" s="29">
+      <c r="BS28" s="24"/>
+      <c r="BT28" s="24"/>
+      <c r="BU28" s="24"/>
+      <c r="BV28" s="22">
         <v>2018</v>
       </c>
-      <c r="BW28" s="30"/>
-      <c r="BX28" s="30"/>
-      <c r="BY28" s="30"/>
-      <c r="BZ28" s="26">
+      <c r="BW28" s="24"/>
+      <c r="BX28" s="24"/>
+      <c r="BY28" s="24"/>
+      <c r="BZ28" s="22">
         <v>2019</v>
       </c>
-      <c r="CA28" s="27"/>
-      <c r="CB28" s="27"/>
-      <c r="CC28" s="27"/>
-      <c r="CD28" s="26">
+      <c r="CA28" s="24"/>
+      <c r="CB28" s="24"/>
+      <c r="CC28" s="24"/>
+      <c r="CD28" s="22">
         <v>2020</v>
       </c>
-      <c r="CE28" s="26"/>
-      <c r="CF28" s="26"/>
-      <c r="CG28" s="26"/>
-      <c r="CH28" s="26">
+      <c r="CE28" s="24"/>
+      <c r="CF28" s="24"/>
+      <c r="CG28" s="24"/>
+      <c r="CH28" s="22">
         <v>2021</v>
       </c>
-      <c r="CI28" s="26"/>
-      <c r="CJ28" s="26"/>
-      <c r="CK28" s="26"/>
-      <c r="CL28" s="25">
+      <c r="CI28" s="22"/>
+      <c r="CJ28" s="22"/>
+      <c r="CK28" s="22"/>
+      <c r="CL28" s="22">
         <v>2022</v>
       </c>
+      <c r="CM28" s="22"/>
     </row>
-    <row r="29" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>4</v>
       </c>
@@ -26031,16 +26022,16 @@
       <c r="BU29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="BV29" s="18" t="s">
+      <c r="BV29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="BW29" s="18" t="s">
+      <c r="BW29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="BX29" s="18" t="s">
+      <c r="BX29" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="BY29" s="18" t="s">
+      <c r="BY29" s="6" t="s">
         <v>9</v>
       </c>
       <c r="BZ29" s="6" t="s">
@@ -26082,11 +26073,14 @@
       <c r="CL29" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="CM29" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="30" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -26306,40 +26300,40 @@
       <c r="BU31" s="15">
         <v>152228.22149744202</v>
       </c>
-      <c r="BV31" s="19">
+      <c r="BV31" s="17">
         <v>149040.10882542259</v>
       </c>
-      <c r="BW31" s="19">
+      <c r="BW31" s="17">
         <v>167337.09472907431</v>
       </c>
-      <c r="BX31" s="19">
+      <c r="BX31" s="17">
         <v>177075.66268935049</v>
       </c>
-      <c r="BY31" s="19">
+      <c r="BY31" s="17">
         <v>157954.57761705143</v>
       </c>
-      <c r="BZ31" s="15">
+      <c r="BZ31" s="17">
         <v>159100.5350056731</v>
       </c>
-      <c r="CA31" s="15">
+      <c r="CA31" s="17">
         <v>177545.41443802236</v>
       </c>
-      <c r="CB31" s="15">
+      <c r="CB31" s="17">
         <v>191392.35613743175</v>
       </c>
-      <c r="CC31" s="15">
+      <c r="CC31" s="17">
         <v>161324.15405450863</v>
       </c>
-      <c r="CD31" s="15">
+      <c r="CD31" s="17">
         <v>147865.98794217067</v>
       </c>
-      <c r="CE31" s="15">
+      <c r="CE31" s="17">
         <v>80442.097894682389</v>
       </c>
-      <c r="CF31" s="15">
+      <c r="CF31" s="17">
         <v>125876.72598385259</v>
       </c>
-      <c r="CG31" s="15">
+      <c r="CG31" s="17">
         <v>118317.68266628485</v>
       </c>
       <c r="CH31" s="15">
@@ -26355,9 +26349,11 @@
         <v>125776.69532565904</v>
       </c>
       <c r="CL31" s="15">
-        <v>131184.29715276285</v>
-      </c>
-      <c r="CM31" s="11"/>
+        <v>125965.53312470275</v>
+      </c>
+      <c r="CM31" s="15">
+        <v>124248.10931907622</v>
+      </c>
       <c r="CN31" s="11"/>
       <c r="CO31" s="11"/>
       <c r="CP31" s="11"/>
@@ -26419,7 +26415,7 @@
       <c r="ET31" s="11"/>
       <c r="EU31" s="11"/>
     </row>
-    <row r="32" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
@@ -26639,40 +26635,40 @@
       <c r="BU32" s="15">
         <v>129623.73104248037</v>
       </c>
-      <c r="BV32" s="19">
+      <c r="BV32" s="17">
         <v>134195.46655524126</v>
       </c>
-      <c r="BW32" s="19">
+      <c r="BW32" s="17">
         <v>135334.25394789461</v>
       </c>
-      <c r="BX32" s="19">
+      <c r="BX32" s="17">
         <v>135526.8404788948</v>
       </c>
-      <c r="BY32" s="19">
+      <c r="BY32" s="17">
         <v>133208.64124452166</v>
       </c>
-      <c r="BZ32" s="15">
+      <c r="BZ32" s="17">
         <v>136972.71021659742</v>
       </c>
-      <c r="CA32" s="15">
+      <c r="CA32" s="17">
         <v>138036.86946670586</v>
       </c>
-      <c r="CB32" s="15">
+      <c r="CB32" s="17">
         <v>138349.08179200045</v>
       </c>
-      <c r="CC32" s="15">
+      <c r="CC32" s="17">
         <v>135748.35967848721</v>
       </c>
-      <c r="CD32" s="15">
+      <c r="CD32" s="17">
         <v>139666.02219371271</v>
       </c>
-      <c r="CE32" s="15">
+      <c r="CE32" s="17">
         <v>140776.89467278705</v>
       </c>
-      <c r="CF32" s="15">
+      <c r="CF32" s="17">
         <v>140615.47266983439</v>
       </c>
-      <c r="CG32" s="15">
+      <c r="CG32" s="17">
         <v>137713.88138289549</v>
       </c>
       <c r="CH32" s="15">
@@ -26690,7 +26686,9 @@
       <c r="CL32" s="15">
         <v>142965.36018506213</v>
       </c>
-      <c r="CM32" s="11"/>
+      <c r="CM32" s="15">
+        <v>144141.52897438855</v>
+      </c>
       <c r="CN32" s="11"/>
       <c r="CO32" s="11"/>
       <c r="CP32" s="11"/>
@@ -26752,7 +26750,7 @@
       <c r="ET32" s="11"/>
       <c r="EU32" s="11"/>
     </row>
-    <row r="33" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -26825,10 +26823,10 @@
       <c r="BS33" s="11"/>
       <c r="BT33" s="11"/>
       <c r="BU33" s="11"/>
-      <c r="BV33" s="20"/>
-      <c r="BW33" s="20"/>
-      <c r="BX33" s="20"/>
-      <c r="BY33" s="20"/>
+      <c r="BV33" s="11"/>
+      <c r="BW33" s="11"/>
+      <c r="BX33" s="11"/>
+      <c r="BY33" s="11"/>
       <c r="BZ33" s="11"/>
       <c r="CA33" s="11"/>
       <c r="CB33" s="11"/>
@@ -26904,7 +26902,7 @@
       <c r="ET33" s="11"/>
       <c r="EU33" s="11"/>
     </row>
-    <row r="34" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>13</v>
       </c>
@@ -27124,40 +27122,40 @@
       <c r="BU34" s="16">
         <v>281851.95253992238</v>
       </c>
-      <c r="BV34" s="21">
+      <c r="BV34" s="18">
         <v>283235.57538066385</v>
       </c>
-      <c r="BW34" s="21">
+      <c r="BW34" s="18">
         <v>302671.34867696895</v>
       </c>
-      <c r="BX34" s="21">
+      <c r="BX34" s="18">
         <v>312602.50316824531</v>
       </c>
-      <c r="BY34" s="21">
+      <c r="BY34" s="18">
         <v>291163.21886157308</v>
       </c>
-      <c r="BZ34" s="16">
+      <c r="BZ34" s="18">
         <v>296073.24522227049</v>
       </c>
-      <c r="CA34" s="16">
+      <c r="CA34" s="18">
         <v>315582.28390472825</v>
       </c>
-      <c r="CB34" s="16">
+      <c r="CB34" s="18">
         <v>329741.4379294322</v>
       </c>
-      <c r="CC34" s="16">
+      <c r="CC34" s="18">
         <v>297072.51373299584</v>
       </c>
-      <c r="CD34" s="16">
+      <c r="CD34" s="18">
         <v>287532.01013588335</v>
       </c>
-      <c r="CE34" s="16">
+      <c r="CE34" s="18">
         <v>221218.99256746942</v>
       </c>
-      <c r="CF34" s="16">
+      <c r="CF34" s="18">
         <v>266492.19865368697</v>
       </c>
-      <c r="CG34" s="16">
+      <c r="CG34" s="18">
         <v>256031.56404918034</v>
       </c>
       <c r="CH34" s="16">
@@ -27173,9 +27171,11 @@
         <v>264807.61897255026</v>
       </c>
       <c r="CL34" s="16">
-        <v>274149.65733782499</v>
-      </c>
-      <c r="CM34" s="11"/>
+        <v>268930.89330976491</v>
+      </c>
+      <c r="CM34" s="16">
+        <v>268389.63829346478</v>
+      </c>
       <c r="CN34" s="11"/>
       <c r="CO34" s="11"/>
       <c r="CP34" s="11"/>
@@ -27237,7 +27237,7 @@
       <c r="ET34" s="11"/>
       <c r="EU34" s="11"/>
     </row>
-    <row r="35" spans="1:151" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:151" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -27311,10 +27311,10 @@
       <c r="BS35" s="9"/>
       <c r="BT35" s="9"/>
       <c r="BU35" s="9"/>
-      <c r="BV35" s="22"/>
-      <c r="BW35" s="22"/>
-      <c r="BX35" s="22"/>
-      <c r="BY35" s="22"/>
+      <c r="BV35" s="9"/>
+      <c r="BW35" s="9"/>
+      <c r="BX35" s="9"/>
+      <c r="BY35" s="9"/>
       <c r="BZ35" s="9"/>
       <c r="CA35" s="9"/>
       <c r="CB35" s="9"/>
@@ -27328,13 +27328,14 @@
       <c r="CJ35" s="9"/>
       <c r="CK35" s="9"/>
       <c r="CL35" s="9"/>
+      <c r="CM35" s="9"/>
     </row>
-    <row r="36" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -27407,10 +27408,10 @@
       <c r="BS37" s="11"/>
       <c r="BT37" s="11"/>
       <c r="BU37" s="11"/>
-      <c r="BV37" s="20"/>
-      <c r="BW37" s="20"/>
-      <c r="BX37" s="20"/>
-      <c r="BY37" s="20"/>
+      <c r="BV37" s="11"/>
+      <c r="BW37" s="11"/>
+      <c r="BX37" s="11"/>
+      <c r="BY37" s="11"/>
       <c r="BZ37" s="11"/>
       <c r="CA37" s="11"/>
       <c r="CB37" s="11"/>
@@ -27486,7 +27487,7 @@
       <c r="ET37" s="11"/>
       <c r="EU37" s="11"/>
     </row>
-    <row r="38" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -27559,10 +27560,10 @@
       <c r="BS38" s="11"/>
       <c r="BT38" s="11"/>
       <c r="BU38" s="11"/>
-      <c r="BV38" s="20"/>
-      <c r="BW38" s="20"/>
-      <c r="BX38" s="20"/>
-      <c r="BY38" s="20"/>
+      <c r="BV38" s="11"/>
+      <c r="BW38" s="11"/>
+      <c r="BX38" s="11"/>
+      <c r="BY38" s="11"/>
       <c r="BZ38" s="11"/>
       <c r="CA38" s="11"/>
       <c r="CB38" s="11"/>
@@ -27638,196 +27639,174 @@
       <c r="ET38" s="11"/>
       <c r="EU38" s="11"/>
     </row>
-    <row r="39" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="CI43" s="32"/>
-      <c r="CJ43" s="32"/>
-      <c r="CK43" s="32"/>
-      <c r="CL43" s="32"/>
-      <c r="CM43" s="32"/>
     </row>
-    <row r="44" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="CI44" s="32"/>
-      <c r="CJ44" s="32"/>
-      <c r="CK44" s="32"/>
-      <c r="CL44" s="32"/>
-      <c r="CM44" s="32"/>
     </row>
-    <row r="45" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="CI45" s="32"/>
-      <c r="CJ45" s="32"/>
-      <c r="CK45" s="32"/>
-      <c r="CL45" s="32"/>
-      <c r="CM45" s="32"/>
     </row>
-    <row r="46" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="CI46" s="32"/>
-      <c r="CJ46" s="32"/>
-      <c r="CK46" s="32"/>
-      <c r="CL46" s="32"/>
-      <c r="CM46" s="32"/>
+    <row r="47" spans="1:151" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="S47" s="22"/>
+      <c r="T47" s="22"/>
+      <c r="U47" s="22"/>
+      <c r="V47" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="W47" s="22"/>
+      <c r="X47" s="22"/>
+      <c r="Y47" s="22"/>
+      <c r="Z47" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA47" s="22"/>
+      <c r="AB47" s="22"/>
+      <c r="AC47" s="22"/>
+      <c r="AD47" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE47" s="22"/>
+      <c r="AF47" s="22"/>
+      <c r="AG47" s="22"/>
+      <c r="AH47" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI47" s="22"/>
+      <c r="AJ47" s="22"/>
+      <c r="AK47" s="22"/>
+      <c r="AL47" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM47" s="22"/>
+      <c r="AN47" s="22"/>
+      <c r="AO47" s="22"/>
+      <c r="AP47" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ47" s="22"/>
+      <c r="AR47" s="22"/>
+      <c r="AS47" s="22"/>
+      <c r="AT47" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU47" s="22"/>
+      <c r="AV47" s="22"/>
+      <c r="AW47" s="22"/>
+      <c r="AX47" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY47" s="22"/>
+      <c r="AZ47" s="22"/>
+      <c r="BA47" s="22"/>
+      <c r="BB47" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC47" s="22"/>
+      <c r="BD47" s="22"/>
+      <c r="BE47" s="22"/>
+      <c r="BF47" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="BG47" s="22"/>
+      <c r="BH47" s="22"/>
+      <c r="BI47" s="22"/>
+      <c r="BJ47" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="BK47" s="22"/>
+      <c r="BL47" s="22"/>
+      <c r="BM47" s="22"/>
+      <c r="BN47" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="BO47" s="22"/>
+      <c r="BP47" s="22"/>
+      <c r="BQ47" s="22"/>
+      <c r="BR47" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="BS47" s="22"/>
+      <c r="BT47" s="22"/>
+      <c r="BU47" s="22"/>
+      <c r="BV47" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="BW47" s="22"/>
+      <c r="BX47" s="22"/>
+      <c r="BY47" s="22"/>
+      <c r="BZ47" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="CA47" s="22"/>
+      <c r="CB47" s="22"/>
+      <c r="CC47" s="22"/>
+      <c r="CD47" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="CE47" s="22"/>
+      <c r="CF47" s="22"/>
+      <c r="CG47" s="22"/>
+      <c r="CH47" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="CI47" s="22"/>
+      <c r="CJ47" s="20"/>
+      <c r="CK47" s="20"/>
+      <c r="CL47" s="19"/>
+      <c r="CM47" s="19"/>
     </row>
-    <row r="47" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="O47" s="26"/>
-      <c r="P47" s="26"/>
-      <c r="Q47" s="26"/>
-      <c r="R47" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="S47" s="26"/>
-      <c r="T47" s="26"/>
-      <c r="U47" s="26"/>
-      <c r="V47" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="W47" s="26"/>
-      <c r="X47" s="26"/>
-      <c r="Y47" s="26"/>
-      <c r="Z47" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA47" s="26"/>
-      <c r="AB47" s="26"/>
-      <c r="AC47" s="26"/>
-      <c r="AD47" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE47" s="26"/>
-      <c r="AF47" s="26"/>
-      <c r="AG47" s="26"/>
-      <c r="AH47" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI47" s="26"/>
-      <c r="AJ47" s="26"/>
-      <c r="AK47" s="26"/>
-      <c r="AL47" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM47" s="26"/>
-      <c r="AN47" s="26"/>
-      <c r="AO47" s="26"/>
-      <c r="AP47" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ47" s="26"/>
-      <c r="AR47" s="26"/>
-      <c r="AS47" s="26"/>
-      <c r="AT47" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU47" s="26"/>
-      <c r="AV47" s="26"/>
-      <c r="AW47" s="26"/>
-      <c r="AX47" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY47" s="26"/>
-      <c r="AZ47" s="26"/>
-      <c r="BA47" s="26"/>
-      <c r="BB47" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC47" s="26"/>
-      <c r="BD47" s="26"/>
-      <c r="BE47" s="26"/>
-      <c r="BF47" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="BG47" s="26"/>
-      <c r="BH47" s="26"/>
-      <c r="BI47" s="26"/>
-      <c r="BJ47" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="BK47" s="26"/>
-      <c r="BL47" s="26"/>
-      <c r="BM47" s="26"/>
-      <c r="BN47" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="BO47" s="26"/>
-      <c r="BP47" s="26"/>
-      <c r="BQ47" s="26"/>
-      <c r="BR47" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="BS47" s="26"/>
-      <c r="BT47" s="26"/>
-      <c r="BU47" s="26"/>
-      <c r="BV47" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="BW47" s="29"/>
-      <c r="BX47" s="29"/>
-      <c r="BY47" s="29"/>
-      <c r="BZ47" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="CA47" s="26"/>
-      <c r="CB47" s="26"/>
-      <c r="CC47" s="26"/>
-      <c r="CD47" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="CE47" s="26"/>
-      <c r="CF47" s="26"/>
-      <c r="CG47" s="26"/>
-      <c r="CH47" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="CI47" s="33"/>
-      <c r="CJ47" s="33"/>
-      <c r="CK47" s="33"/>
-      <c r="CL47" s="34"/>
-      <c r="CM47" s="32"/>
-    </row>
-    <row r="48" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>4</v>
       </c>
@@ -28047,16 +28026,16 @@
       <c r="BU48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="BV48" s="23" t="s">
+      <c r="BV48" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="BW48" s="23" t="s">
+      <c r="BW48" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BX48" s="23" t="s">
+      <c r="BX48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="BY48" s="23" t="s">
+      <c r="BY48" s="5" t="s">
         <v>9</v>
       </c>
       <c r="BZ48" s="5" t="s">
@@ -28086,21 +28065,18 @@
       <c r="CH48" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="CI48" s="33"/>
-      <c r="CJ48" s="33"/>
-      <c r="CK48" s="33"/>
-      <c r="CL48" s="33"/>
-      <c r="CM48" s="32"/>
+      <c r="CI48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="CJ48" s="5"/>
+      <c r="CK48" s="5"/>
+      <c r="CL48" s="5"/>
+      <c r="CM48" s="21"/>
     </row>
-    <row r="49" spans="1:147" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:147" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="CI49" s="32"/>
-      <c r="CJ49" s="32"/>
-      <c r="CK49" s="32"/>
-      <c r="CL49" s="32"/>
-      <c r="CM49" s="32"/>
     </row>
-    <row r="50" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:147" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>11</v>
       </c>
@@ -28320,16 +28296,16 @@
       <c r="BU50" s="12">
         <v>10.563571477456676</v>
       </c>
-      <c r="BV50" s="24">
+      <c r="BV50" s="12">
         <v>9.6806316195680466</v>
       </c>
-      <c r="BW50" s="24">
+      <c r="BW50" s="12">
         <v>6.9478970539928184</v>
       </c>
-      <c r="BX50" s="24">
+      <c r="BX50" s="12">
         <v>7.1302579747115686</v>
       </c>
-      <c r="BY50" s="24">
+      <c r="BY50" s="12">
         <v>1.3729005017420803</v>
       </c>
       <c r="BZ50" s="12">
@@ -28357,13 +28333,15 @@
         <v>11.195427327526716</v>
       </c>
       <c r="CH50" s="12">
-        <v>20.249971507419957</v>
-      </c>
-      <c r="CI50" s="35"/>
-      <c r="CJ50" s="35"/>
-      <c r="CK50" s="35"/>
-      <c r="CL50" s="35"/>
-      <c r="CM50" s="35"/>
+        <v>15.466196015240513</v>
+      </c>
+      <c r="CI50" s="12">
+        <v>12.937920429493062</v>
+      </c>
+      <c r="CJ50" s="12"/>
+      <c r="CK50" s="12"/>
+      <c r="CL50" s="12"/>
+      <c r="CM50" s="11"/>
       <c r="CN50" s="11"/>
       <c r="CO50" s="11"/>
       <c r="CP50" s="11"/>
@@ -28421,7 +28399,7 @@
       <c r="EP50" s="11"/>
       <c r="EQ50" s="11"/>
     </row>
-    <row r="51" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:147" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
@@ -28641,16 +28619,16 @@
       <c r="BU51" s="12">
         <v>6.7075390002172384</v>
       </c>
-      <c r="BV51" s="24">
+      <c r="BV51" s="12">
         <v>5.0977626318906601</v>
       </c>
-      <c r="BW51" s="24">
+      <c r="BW51" s="12">
         <v>4.5662544107340182</v>
       </c>
-      <c r="BX51" s="24">
+      <c r="BX51" s="12">
         <v>4.8593849301118155</v>
       </c>
-      <c r="BY51" s="24">
+      <c r="BY51" s="12">
         <v>4.3340476321099572</v>
       </c>
       <c r="BZ51" s="12">
@@ -28680,11 +28658,13 @@
       <c r="CH51" s="12">
         <v>2.2838921682917288</v>
       </c>
-      <c r="CI51" s="35"/>
-      <c r="CJ51" s="35"/>
-      <c r="CK51" s="35"/>
-      <c r="CL51" s="35"/>
-      <c r="CM51" s="35"/>
+      <c r="CI51" s="12">
+        <v>2.4905148435179711</v>
+      </c>
+      <c r="CJ51" s="12"/>
+      <c r="CK51" s="12"/>
+      <c r="CL51" s="12"/>
+      <c r="CM51" s="11"/>
       <c r="CN51" s="11"/>
       <c r="CO51" s="11"/>
       <c r="CP51" s="11"/>
@@ -28742,7 +28722,7 @@
       <c r="EP51" s="11"/>
       <c r="EQ51" s="11"/>
     </row>
-    <row r="52" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:147" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -28816,10 +28796,10 @@
       <c r="BS52" s="11"/>
       <c r="BT52" s="11"/>
       <c r="BU52" s="11"/>
-      <c r="BV52" s="20"/>
-      <c r="BW52" s="20"/>
-      <c r="BX52" s="20"/>
-      <c r="BY52" s="20"/>
+      <c r="BV52" s="11"/>
+      <c r="BW52" s="11"/>
+      <c r="BX52" s="11"/>
+      <c r="BY52" s="11"/>
       <c r="BZ52" s="11"/>
       <c r="CA52" s="11"/>
       <c r="CB52" s="11"/>
@@ -28829,11 +28809,11 @@
       <c r="CF52" s="11"/>
       <c r="CG52" s="11"/>
       <c r="CH52" s="11"/>
-      <c r="CI52" s="35"/>
-      <c r="CJ52" s="35"/>
-      <c r="CK52" s="35"/>
-      <c r="CL52" s="35"/>
-      <c r="CM52" s="35"/>
+      <c r="CI52" s="11"/>
+      <c r="CJ52" s="11"/>
+      <c r="CK52" s="11"/>
+      <c r="CL52" s="11"/>
+      <c r="CM52" s="11"/>
       <c r="CN52" s="11"/>
       <c r="CO52" s="11"/>
       <c r="CP52" s="11"/>
@@ -28891,7 +28871,7 @@
       <c r="EP52" s="11"/>
       <c r="EQ52" s="11"/>
     </row>
-    <row r="53" spans="1:147" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:147" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>13</v>
       </c>
@@ -29111,16 +29091,16 @@
       <c r="BU53" s="12">
         <v>8.7748897057317237</v>
       </c>
-      <c r="BV53" s="24">
+      <c r="BV53" s="12">
         <v>7.5142356164854078</v>
       </c>
-      <c r="BW53" s="24">
+      <c r="BW53" s="12">
         <v>5.8832621192702987</v>
       </c>
-      <c r="BX53" s="24">
+      <c r="BX53" s="12">
         <v>6.1373917669679656</v>
       </c>
-      <c r="BY53" s="24">
+      <c r="BY53" s="12">
         <v>2.7203696708347564</v>
       </c>
       <c r="BZ53" s="12">
@@ -29148,13 +29128,15 @@
         <v>6.3503652909170825</v>
       </c>
       <c r="CH53" s="12">
-        <v>10.40464227288038</v>
-      </c>
-      <c r="CI53" s="35"/>
-      <c r="CJ53" s="35"/>
-      <c r="CK53" s="35"/>
-      <c r="CL53" s="35"/>
-      <c r="CM53" s="35"/>
+        <v>8.2423538517311812</v>
+      </c>
+      <c r="CI53" s="12">
+        <v>7.2098278687646342</v>
+      </c>
+      <c r="CJ53" s="12"/>
+      <c r="CK53" s="12"/>
+      <c r="CL53" s="12"/>
+      <c r="CM53" s="11"/>
       <c r="CN53" s="11"/>
       <c r="CO53" s="11"/>
       <c r="CP53" s="11"/>
@@ -29212,7 +29194,7 @@
       <c r="EP53" s="11"/>
       <c r="EQ53" s="11"/>
     </row>
-    <row r="54" spans="1:147" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:147" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -29286,10 +29268,10 @@
       <c r="BS54" s="9"/>
       <c r="BT54" s="9"/>
       <c r="BU54" s="9"/>
-      <c r="BV54" s="22"/>
-      <c r="BW54" s="22"/>
-      <c r="BX54" s="22"/>
-      <c r="BY54" s="22"/>
+      <c r="BV54" s="9"/>
+      <c r="BW54" s="9"/>
+      <c r="BX54" s="9"/>
+      <c r="BY54" s="9"/>
       <c r="BZ54" s="9"/>
       <c r="CA54" s="9"/>
       <c r="CB54" s="9"/>
@@ -29299,23 +29281,18 @@
       <c r="CF54" s="9"/>
       <c r="CG54" s="9"/>
       <c r="CH54" s="9"/>
-      <c r="CI54" s="36"/>
-      <c r="CJ54" s="36"/>
-      <c r="CK54" s="36"/>
-      <c r="CL54" s="36"/>
-      <c r="CM54" s="32"/>
+      <c r="CI54" s="9"/>
+      <c r="CJ54" s="9"/>
+      <c r="CK54" s="9"/>
+      <c r="CL54" s="9"/>
+      <c r="CM54" s="9"/>
     </row>
-    <row r="55" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="CI55" s="32"/>
-      <c r="CJ55" s="32"/>
-      <c r="CK55" s="32"/>
-      <c r="CL55" s="32"/>
-      <c r="CM55" s="32"/>
     </row>
-    <row r="56" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:147" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -29388,10 +29365,10 @@
       <c r="BS56" s="11"/>
       <c r="BT56" s="11"/>
       <c r="BU56" s="11"/>
-      <c r="BV56" s="20"/>
-      <c r="BW56" s="20"/>
-      <c r="BX56" s="20"/>
-      <c r="BY56" s="20"/>
+      <c r="BV56" s="11"/>
+      <c r="BW56" s="11"/>
+      <c r="BX56" s="11"/>
+      <c r="BY56" s="11"/>
       <c r="BZ56" s="11"/>
       <c r="CA56" s="11"/>
       <c r="CB56" s="11"/>
@@ -29401,11 +29378,11 @@
       <c r="CF56" s="11"/>
       <c r="CG56" s="11"/>
       <c r="CH56" s="11"/>
-      <c r="CI56" s="35"/>
-      <c r="CJ56" s="35"/>
-      <c r="CK56" s="35"/>
-      <c r="CL56" s="35"/>
-      <c r="CM56" s="35"/>
+      <c r="CI56" s="11"/>
+      <c r="CJ56" s="11"/>
+      <c r="CK56" s="11"/>
+      <c r="CL56" s="11"/>
+      <c r="CM56" s="11"/>
       <c r="CN56" s="11"/>
       <c r="CO56" s="11"/>
       <c r="CP56" s="11"/>
@@ -29463,7 +29440,7 @@
       <c r="EP56" s="11"/>
       <c r="EQ56" s="11"/>
     </row>
-    <row r="57" spans="1:147" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:147" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
@@ -29536,10 +29513,10 @@
       <c r="BS57" s="11"/>
       <c r="BT57" s="11"/>
       <c r="BU57" s="11"/>
-      <c r="BV57" s="20"/>
-      <c r="BW57" s="20"/>
-      <c r="BX57" s="20"/>
-      <c r="BY57" s="20"/>
+      <c r="BV57" s="11"/>
+      <c r="BW57" s="11"/>
+      <c r="BX57" s="11"/>
+      <c r="BY57" s="11"/>
       <c r="BZ57" s="11"/>
       <c r="CA57" s="11"/>
       <c r="CB57" s="11"/>
@@ -29549,11 +29526,11 @@
       <c r="CF57" s="11"/>
       <c r="CG57" s="11"/>
       <c r="CH57" s="11"/>
-      <c r="CI57" s="35"/>
-      <c r="CJ57" s="35"/>
-      <c r="CK57" s="35"/>
-      <c r="CL57" s="35"/>
-      <c r="CM57" s="35"/>
+      <c r="CI57" s="11"/>
+      <c r="CJ57" s="11"/>
+      <c r="CK57" s="11"/>
+      <c r="CL57" s="11"/>
+      <c r="CM57" s="11"/>
       <c r="CN57" s="11"/>
       <c r="CO57" s="11"/>
       <c r="CP57" s="11"/>
@@ -29611,204 +29588,174 @@
       <c r="EP57" s="11"/>
       <c r="EQ57" s="11"/>
     </row>
-    <row r="58" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="CI58" s="32"/>
-      <c r="CJ58" s="32"/>
-      <c r="CK58" s="32"/>
-      <c r="CL58" s="32"/>
-      <c r="CM58" s="32"/>
     </row>
-    <row r="59" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="CI59" s="32"/>
-      <c r="CJ59" s="32"/>
-      <c r="CK59" s="32"/>
-      <c r="CL59" s="32"/>
-      <c r="CM59" s="32"/>
     </row>
-    <row r="60" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="CI60" s="32"/>
-      <c r="CJ60" s="32"/>
-      <c r="CK60" s="32"/>
-      <c r="CL60" s="32"/>
-      <c r="CM60" s="32"/>
     </row>
-    <row r="62" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:147" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:147" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="CI64" s="32"/>
-      <c r="CJ64" s="32"/>
-      <c r="CK64" s="32"/>
-      <c r="CL64" s="32"/>
-      <c r="CM64" s="32"/>
-      <c r="CN64" s="32"/>
     </row>
-    <row r="65" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="CI65" s="32"/>
-      <c r="CJ65" s="32"/>
-      <c r="CK65" s="32"/>
-      <c r="CL65" s="32"/>
-      <c r="CM65" s="32"/>
-      <c r="CN65" s="32"/>
+    <row r="66" spans="1:151" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="23"/>
+      <c r="N66" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O66" s="23"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="S66" s="23"/>
+      <c r="T66" s="23"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="W66" s="23"/>
+      <c r="X66" s="23"/>
+      <c r="Y66" s="23"/>
+      <c r="Z66" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA66" s="23"/>
+      <c r="AB66" s="23"/>
+      <c r="AC66" s="23"/>
+      <c r="AD66" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE66" s="23"/>
+      <c r="AF66" s="23"/>
+      <c r="AG66" s="23"/>
+      <c r="AH66" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI66" s="23"/>
+      <c r="AJ66" s="23"/>
+      <c r="AK66" s="23"/>
+      <c r="AL66" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM66" s="23"/>
+      <c r="AN66" s="23"/>
+      <c r="AO66" s="23"/>
+      <c r="AP66" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ66" s="23"/>
+      <c r="AR66" s="23"/>
+      <c r="AS66" s="23"/>
+      <c r="AT66" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU66" s="23"/>
+      <c r="AV66" s="23"/>
+      <c r="AW66" s="23"/>
+      <c r="AX66" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY66" s="23"/>
+      <c r="AZ66" s="23"/>
+      <c r="BA66" s="23"/>
+      <c r="BB66" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC66" s="23"/>
+      <c r="BD66" s="23"/>
+      <c r="BE66" s="23"/>
+      <c r="BF66" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="BG66" s="23"/>
+      <c r="BH66" s="23"/>
+      <c r="BI66" s="23"/>
+      <c r="BJ66" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="BK66" s="23"/>
+      <c r="BL66" s="23"/>
+      <c r="BM66" s="23"/>
+      <c r="BN66" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="BO66" s="23"/>
+      <c r="BP66" s="23"/>
+      <c r="BQ66" s="23"/>
+      <c r="BR66" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="BS66" s="23"/>
+      <c r="BT66" s="23"/>
+      <c r="BU66" s="23"/>
+      <c r="BV66" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="BW66" s="23"/>
+      <c r="BX66" s="23"/>
+      <c r="BY66" s="23"/>
+      <c r="BZ66" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="CA66" s="23"/>
+      <c r="CB66" s="23"/>
+      <c r="CC66" s="23"/>
+      <c r="CD66" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="CE66" s="23"/>
+      <c r="CF66" s="23"/>
+      <c r="CG66" s="23"/>
+      <c r="CH66" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="CI66" s="22"/>
+      <c r="CJ66" s="20"/>
+      <c r="CK66" s="20"/>
+      <c r="CL66" s="19"/>
+      <c r="CM66" s="19"/>
     </row>
-    <row r="66" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="A66" s="4"/>
-      <c r="B66" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="K66" s="28"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="28"/>
-      <c r="N66" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="O66" s="28"/>
-      <c r="P66" s="28"/>
-      <c r="Q66" s="28"/>
-      <c r="R66" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="S66" s="28"/>
-      <c r="T66" s="28"/>
-      <c r="U66" s="28"/>
-      <c r="V66" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="W66" s="28"/>
-      <c r="X66" s="28"/>
-      <c r="Y66" s="28"/>
-      <c r="Z66" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA66" s="28"/>
-      <c r="AB66" s="28"/>
-      <c r="AC66" s="28"/>
-      <c r="AD66" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE66" s="28"/>
-      <c r="AF66" s="28"/>
-      <c r="AG66" s="28"/>
-      <c r="AH66" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI66" s="28"/>
-      <c r="AJ66" s="28"/>
-      <c r="AK66" s="28"/>
-      <c r="AL66" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM66" s="28"/>
-      <c r="AN66" s="28"/>
-      <c r="AO66" s="28"/>
-      <c r="AP66" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ66" s="28"/>
-      <c r="AR66" s="28"/>
-      <c r="AS66" s="28"/>
-      <c r="AT66" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU66" s="28"/>
-      <c r="AV66" s="28"/>
-      <c r="AW66" s="28"/>
-      <c r="AX66" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY66" s="28"/>
-      <c r="AZ66" s="28"/>
-      <c r="BA66" s="28"/>
-      <c r="BB66" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC66" s="28"/>
-      <c r="BD66" s="28"/>
-      <c r="BE66" s="28"/>
-      <c r="BF66" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="BG66" s="28"/>
-      <c r="BH66" s="28"/>
-      <c r="BI66" s="28"/>
-      <c r="BJ66" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="BK66" s="28"/>
-      <c r="BL66" s="28"/>
-      <c r="BM66" s="28"/>
-      <c r="BN66" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="BO66" s="28"/>
-      <c r="BP66" s="28"/>
-      <c r="BQ66" s="28"/>
-      <c r="BR66" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="BS66" s="28"/>
-      <c r="BT66" s="28"/>
-      <c r="BU66" s="28"/>
-      <c r="BV66" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="BW66" s="31"/>
-      <c r="BX66" s="31"/>
-      <c r="BY66" s="31"/>
-      <c r="BZ66" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="CA66" s="26"/>
-      <c r="CB66" s="26"/>
-      <c r="CC66" s="26"/>
-      <c r="CD66" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="CE66" s="26"/>
-      <c r="CF66" s="26"/>
-      <c r="CG66" s="26"/>
-      <c r="CH66" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="CI66" s="33"/>
-      <c r="CJ66" s="33"/>
-      <c r="CK66" s="33"/>
-      <c r="CL66" s="34"/>
-      <c r="CM66" s="32"/>
-      <c r="CN66" s="32"/>
-    </row>
-    <row r="67" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>4</v>
       </c>
@@ -30028,16 +29975,16 @@
       <c r="BU67" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="BV67" s="23" t="s">
+      <c r="BV67" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="BW67" s="23" t="s">
+      <c r="BW67" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BX67" s="23" t="s">
+      <c r="BX67" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="BY67" s="23" t="s">
+      <c r="BY67" s="5" t="s">
         <v>9</v>
       </c>
       <c r="BZ67" s="5" t="s">
@@ -30067,23 +30014,18 @@
       <c r="CH67" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="CI67" s="33"/>
-      <c r="CJ67" s="33"/>
-      <c r="CK67" s="33"/>
-      <c r="CL67" s="33"/>
-      <c r="CM67" s="32"/>
-      <c r="CN67" s="32"/>
+      <c r="CI67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="CJ67" s="5"/>
+      <c r="CK67" s="5"/>
+      <c r="CL67" s="5"/>
+      <c r="CM67" s="21"/>
     </row>
-    <row r="68" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
-      <c r="CI68" s="32"/>
-      <c r="CJ68" s="32"/>
-      <c r="CK68" s="32"/>
-      <c r="CL68" s="32"/>
-      <c r="CM68" s="32"/>
-      <c r="CN68" s="32"/>
     </row>
-    <row r="69" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>11</v>
       </c>
@@ -30303,16 +30245,16 @@
       <c r="BU69" s="12">
         <v>3.7616915334622405</v>
       </c>
-      <c r="BV69" s="24">
+      <c r="BV69" s="12">
         <v>6.7501468292905855</v>
       </c>
-      <c r="BW69" s="24">
+      <c r="BW69" s="12">
         <v>6.1004523387212686</v>
       </c>
-      <c r="BX69" s="24">
+      <c r="BX69" s="12">
         <v>8.0850712235918536</v>
       </c>
-      <c r="BY69" s="24">
+      <c r="BY69" s="12">
         <v>2.1332565907817411</v>
       </c>
       <c r="BZ69" s="12">
@@ -30340,14 +30282,16 @@
         <v>6.3042247712139101</v>
       </c>
       <c r="CH69" s="12">
-        <v>16.399300697350071</v>
-      </c>
-      <c r="CI69" s="35"/>
-      <c r="CJ69" s="35"/>
-      <c r="CK69" s="35"/>
-      <c r="CL69" s="35"/>
-      <c r="CM69" s="35"/>
-      <c r="CN69" s="35"/>
+        <v>11.768712307161124</v>
+      </c>
+      <c r="CI69" s="12">
+        <v>7.1189918961674294</v>
+      </c>
+      <c r="CJ69" s="12"/>
+      <c r="CK69" s="12"/>
+      <c r="CL69" s="12"/>
+      <c r="CM69" s="11"/>
+      <c r="CN69" s="11"/>
       <c r="CO69" s="11"/>
       <c r="CP69" s="11"/>
       <c r="CQ69" s="11"/>
@@ -30404,7 +30348,7 @@
       <c r="EP69" s="11"/>
       <c r="EQ69" s="11"/>
     </row>
-    <row r="70" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>12</v>
       </c>
@@ -30624,16 +30568,16 @@
       <c r="BU70" s="12">
         <v>2.7656280013004846</v>
       </c>
-      <c r="BV70" s="24">
+      <c r="BV70" s="12">
         <v>2.0695510307815965</v>
       </c>
-      <c r="BW70" s="24">
+      <c r="BW70" s="12">
         <v>1.9969929563078637</v>
       </c>
-      <c r="BX70" s="24">
+      <c r="BX70" s="12">
         <v>2.0824224213691167</v>
       </c>
-      <c r="BY70" s="24">
+      <c r="BY70" s="12">
         <v>1.9065718336572388</v>
       </c>
       <c r="BZ70" s="12">
@@ -30663,12 +30607,14 @@
       <c r="CH70" s="12">
         <v>1.1733626980431069</v>
       </c>
-      <c r="CI70" s="35"/>
-      <c r="CJ70" s="35"/>
-      <c r="CK70" s="35"/>
-      <c r="CL70" s="35"/>
-      <c r="CM70" s="35"/>
-      <c r="CN70" s="35"/>
+      <c r="CI70" s="12">
+        <v>1.2723659858168617</v>
+      </c>
+      <c r="CJ70" s="12"/>
+      <c r="CK70" s="12"/>
+      <c r="CL70" s="12"/>
+      <c r="CM70" s="11"/>
+      <c r="CN70" s="11"/>
       <c r="CO70" s="11"/>
       <c r="CP70" s="11"/>
       <c r="CQ70" s="11"/>
@@ -30725,7 +30671,7 @@
       <c r="EP70" s="11"/>
       <c r="EQ70" s="11"/>
     </row>
-    <row r="71" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
@@ -30798,10 +30744,10 @@
       <c r="BS71" s="11"/>
       <c r="BT71" s="11"/>
       <c r="BU71" s="11"/>
-      <c r="BV71" s="20"/>
-      <c r="BW71" s="20"/>
-      <c r="BX71" s="20"/>
-      <c r="BY71" s="20"/>
+      <c r="BV71" s="11"/>
+      <c r="BW71" s="11"/>
+      <c r="BX71" s="11"/>
+      <c r="BY71" s="11"/>
       <c r="BZ71" s="11"/>
       <c r="CA71" s="11"/>
       <c r="CB71" s="11"/>
@@ -30811,12 +30757,12 @@
       <c r="CF71" s="11"/>
       <c r="CG71" s="11"/>
       <c r="CH71" s="11"/>
-      <c r="CI71" s="35"/>
-      <c r="CJ71" s="35"/>
-      <c r="CK71" s="35"/>
-      <c r="CL71" s="35"/>
-      <c r="CM71" s="35"/>
-      <c r="CN71" s="35"/>
+      <c r="CI71" s="11"/>
+      <c r="CJ71" s="11"/>
+      <c r="CK71" s="11"/>
+      <c r="CL71" s="11"/>
+      <c r="CM71" s="11"/>
+      <c r="CN71" s="11"/>
       <c r="CO71" s="11"/>
       <c r="CP71" s="11"/>
       <c r="CQ71" s="11"/>
@@ -30873,7 +30819,7 @@
       <c r="EP71" s="11"/>
       <c r="EQ71" s="11"/>
     </row>
-    <row r="72" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>13</v>
       </c>
@@ -31093,16 +31039,16 @@
       <c r="BU72" s="12">
         <v>3.3036018511639895</v>
       </c>
-      <c r="BV72" s="24">
+      <c r="BV72" s="12">
         <v>4.5325061388750356</v>
       </c>
-      <c r="BW72" s="24">
+      <c r="BW72" s="12">
         <v>4.2656615117999479</v>
       </c>
-      <c r="BX72" s="24">
+      <c r="BX72" s="12">
         <v>5.4826607552667497</v>
       </c>
-      <c r="BY72" s="24">
+      <c r="BY72" s="12">
         <v>2.0295471710086446</v>
       </c>
       <c r="BZ72" s="12">
@@ -31130,14 +31076,16 @@
         <v>3.4277238261467602</v>
       </c>
       <c r="CH72" s="12">
-        <v>7.9289943480642933</v>
-      </c>
-      <c r="CI72" s="35"/>
-      <c r="CJ72" s="35"/>
-      <c r="CK72" s="35"/>
-      <c r="CL72" s="35"/>
-      <c r="CM72" s="35"/>
-      <c r="CN72" s="35"/>
+        <v>5.8744378742099599</v>
+      </c>
+      <c r="CI72" s="12">
+        <v>3.8976022748186523</v>
+      </c>
+      <c r="CJ72" s="12"/>
+      <c r="CK72" s="12"/>
+      <c r="CL72" s="12"/>
+      <c r="CM72" s="11"/>
+      <c r="CN72" s="11"/>
       <c r="CO72" s="11"/>
       <c r="CP72" s="11"/>
       <c r="CQ72" s="11"/>
@@ -31194,7 +31142,7 @@
       <c r="EP72" s="11"/>
       <c r="EQ72" s="11"/>
     </row>
-    <row r="73" spans="1:151" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:151" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -31268,10 +31216,10 @@
       <c r="BS73" s="9"/>
       <c r="BT73" s="9"/>
       <c r="BU73" s="9"/>
-      <c r="BV73" s="22"/>
-      <c r="BW73" s="22"/>
-      <c r="BX73" s="22"/>
-      <c r="BY73" s="22"/>
+      <c r="BV73" s="9"/>
+      <c r="BW73" s="9"/>
+      <c r="BX73" s="9"/>
+      <c r="BY73" s="9"/>
       <c r="BZ73" s="9"/>
       <c r="CA73" s="9"/>
       <c r="CB73" s="9"/>
@@ -31281,25 +31229,18 @@
       <c r="CF73" s="9"/>
       <c r="CG73" s="9"/>
       <c r="CH73" s="9"/>
-      <c r="CI73" s="36"/>
-      <c r="CJ73" s="36"/>
-      <c r="CK73" s="36"/>
-      <c r="CL73" s="36"/>
-      <c r="CM73" s="32"/>
-      <c r="CN73" s="32"/>
+      <c r="CI73" s="9"/>
+      <c r="CJ73" s="9"/>
+      <c r="CK73" s="9"/>
+      <c r="CL73" s="9"/>
+      <c r="CM73" s="9"/>
     </row>
-    <row r="74" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="CI74" s="32"/>
-      <c r="CJ74" s="32"/>
-      <c r="CK74" s="32"/>
-      <c r="CL74" s="32"/>
-      <c r="CM74" s="32"/>
-      <c r="CN74" s="32"/>
     </row>
-    <row r="75" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -31372,10 +31313,10 @@
       <c r="BS75" s="11"/>
       <c r="BT75" s="11"/>
       <c r="BU75" s="11"/>
-      <c r="BV75" s="20"/>
-      <c r="BW75" s="20"/>
-      <c r="BX75" s="20"/>
-      <c r="BY75" s="20"/>
+      <c r="BV75" s="11"/>
+      <c r="BW75" s="11"/>
+      <c r="BX75" s="11"/>
+      <c r="BY75" s="11"/>
       <c r="BZ75" s="11"/>
       <c r="CA75" s="11"/>
       <c r="CB75" s="11"/>
@@ -31385,12 +31326,12 @@
       <c r="CF75" s="11"/>
       <c r="CG75" s="11"/>
       <c r="CH75" s="11"/>
-      <c r="CI75" s="35"/>
-      <c r="CJ75" s="35"/>
-      <c r="CK75" s="35"/>
-      <c r="CL75" s="35"/>
-      <c r="CM75" s="35"/>
-      <c r="CN75" s="35"/>
+      <c r="CI75" s="11"/>
+      <c r="CJ75" s="11"/>
+      <c r="CK75" s="11"/>
+      <c r="CL75" s="11"/>
+      <c r="CM75" s="11"/>
+      <c r="CN75" s="11"/>
       <c r="CO75" s="11"/>
       <c r="CP75" s="11"/>
       <c r="CQ75" s="11"/>
@@ -31447,7 +31388,7 @@
       <c r="EP75" s="11"/>
       <c r="EQ75" s="11"/>
     </row>
-    <row r="76" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -31520,10 +31461,10 @@
       <c r="BS76" s="11"/>
       <c r="BT76" s="11"/>
       <c r="BU76" s="11"/>
-      <c r="BV76" s="20"/>
-      <c r="BW76" s="20"/>
-      <c r="BX76" s="20"/>
-      <c r="BY76" s="20"/>
+      <c r="BV76" s="11"/>
+      <c r="BW76" s="11"/>
+      <c r="BX76" s="11"/>
+      <c r="BY76" s="11"/>
       <c r="BZ76" s="11"/>
       <c r="CA76" s="11"/>
       <c r="CB76" s="11"/>
@@ -31533,12 +31474,12 @@
       <c r="CF76" s="11"/>
       <c r="CG76" s="11"/>
       <c r="CH76" s="11"/>
-      <c r="CI76" s="35"/>
-      <c r="CJ76" s="35"/>
-      <c r="CK76" s="35"/>
-      <c r="CL76" s="35"/>
-      <c r="CM76" s="35"/>
-      <c r="CN76" s="35"/>
+      <c r="CI76" s="11"/>
+      <c r="CJ76" s="11"/>
+      <c r="CK76" s="11"/>
+      <c r="CL76" s="11"/>
+      <c r="CM76" s="11"/>
+      <c r="CN76" s="11"/>
       <c r="CO76" s="11"/>
       <c r="CP76" s="11"/>
       <c r="CQ76" s="11"/>
@@ -31599,196 +31540,171 @@
       <c r="ET76" s="11"/>
       <c r="EU76" s="11"/>
     </row>
-    <row r="77" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="CI77" s="32"/>
-      <c r="CJ77" s="32"/>
-      <c r="CK77" s="32"/>
-      <c r="CL77" s="32"/>
-      <c r="CM77" s="32"/>
-      <c r="CN77" s="32"/>
     </row>
-    <row r="78" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="CI78" s="32"/>
-      <c r="CJ78" s="32"/>
-      <c r="CK78" s="32"/>
-      <c r="CL78" s="32"/>
-      <c r="CM78" s="32"/>
-      <c r="CN78" s="32"/>
     </row>
-    <row r="79" spans="1:151" x14ac:dyDescent="0.2">
-      <c r="CI79" s="32"/>
-      <c r="CJ79" s="32"/>
-      <c r="CK79" s="32"/>
-      <c r="CL79" s="32"/>
-      <c r="CM79" s="32"/>
-      <c r="CN79" s="32"/>
-    </row>
-    <row r="80" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="CI80" s="32"/>
-      <c r="CJ80" s="32"/>
-      <c r="CK80" s="32"/>
-      <c r="CL80" s="32"/>
-      <c r="CM80" s="32"/>
-      <c r="CN80" s="32"/>
     </row>
-    <row r="81" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
-      <c r="B84" s="26">
+      <c r="B84" s="22">
         <v>2000</v>
       </c>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="26">
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="22">
         <v>2001</v>
       </c>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
-      <c r="I84" s="27"/>
-      <c r="J84" s="26">
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="22">
         <v>2002</v>
       </c>
-      <c r="K84" s="27"/>
-      <c r="L84" s="27"/>
-      <c r="M84" s="27"/>
-      <c r="N84" s="26">
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="22">
         <v>2003</v>
       </c>
-      <c r="O84" s="27"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="27"/>
-      <c r="R84" s="26">
+      <c r="O84" s="24"/>
+      <c r="P84" s="24"/>
+      <c r="Q84" s="24"/>
+      <c r="R84" s="22">
         <v>2004</v>
       </c>
-      <c r="S84" s="27"/>
-      <c r="T84" s="27"/>
-      <c r="U84" s="27"/>
-      <c r="V84" s="26">
+      <c r="S84" s="24"/>
+      <c r="T84" s="24"/>
+      <c r="U84" s="24"/>
+      <c r="V84" s="22">
         <v>2005</v>
       </c>
-      <c r="W84" s="27"/>
-      <c r="X84" s="27"/>
-      <c r="Y84" s="27"/>
-      <c r="Z84" s="26">
+      <c r="W84" s="24"/>
+      <c r="X84" s="24"/>
+      <c r="Y84" s="24"/>
+      <c r="Z84" s="22">
         <v>2006</v>
       </c>
-      <c r="AA84" s="27"/>
-      <c r="AB84" s="27"/>
-      <c r="AC84" s="27"/>
-      <c r="AD84" s="26">
+      <c r="AA84" s="24"/>
+      <c r="AB84" s="24"/>
+      <c r="AC84" s="24"/>
+      <c r="AD84" s="22">
         <v>2007</v>
       </c>
-      <c r="AE84" s="27"/>
-      <c r="AF84" s="27"/>
-      <c r="AG84" s="27"/>
-      <c r="AH84" s="26">
+      <c r="AE84" s="24"/>
+      <c r="AF84" s="24"/>
+      <c r="AG84" s="24"/>
+      <c r="AH84" s="22">
         <v>2008</v>
       </c>
-      <c r="AI84" s="27"/>
-      <c r="AJ84" s="27"/>
-      <c r="AK84" s="27"/>
-      <c r="AL84" s="26">
+      <c r="AI84" s="24"/>
+      <c r="AJ84" s="24"/>
+      <c r="AK84" s="24"/>
+      <c r="AL84" s="22">
         <v>2009</v>
       </c>
-      <c r="AM84" s="27"/>
-      <c r="AN84" s="27"/>
-      <c r="AO84" s="27"/>
-      <c r="AP84" s="26">
+      <c r="AM84" s="24"/>
+      <c r="AN84" s="24"/>
+      <c r="AO84" s="24"/>
+      <c r="AP84" s="22">
         <v>2010</v>
       </c>
-      <c r="AQ84" s="27"/>
-      <c r="AR84" s="27"/>
-      <c r="AS84" s="27"/>
-      <c r="AT84" s="26">
+      <c r="AQ84" s="24"/>
+      <c r="AR84" s="24"/>
+      <c r="AS84" s="24"/>
+      <c r="AT84" s="22">
         <v>2011</v>
       </c>
-      <c r="AU84" s="27"/>
-      <c r="AV84" s="27"/>
-      <c r="AW84" s="27"/>
-      <c r="AX84" s="26">
+      <c r="AU84" s="24"/>
+      <c r="AV84" s="24"/>
+      <c r="AW84" s="24"/>
+      <c r="AX84" s="22">
         <v>2012</v>
       </c>
-      <c r="AY84" s="27"/>
-      <c r="AZ84" s="27"/>
-      <c r="BA84" s="27"/>
-      <c r="BB84" s="26">
+      <c r="AY84" s="24"/>
+      <c r="AZ84" s="24"/>
+      <c r="BA84" s="24"/>
+      <c r="BB84" s="22">
         <v>2013</v>
       </c>
-      <c r="BC84" s="27"/>
-      <c r="BD84" s="27"/>
-      <c r="BE84" s="27"/>
-      <c r="BF84" s="26">
+      <c r="BC84" s="24"/>
+      <c r="BD84" s="24"/>
+      <c r="BE84" s="24"/>
+      <c r="BF84" s="22">
         <v>2014</v>
       </c>
-      <c r="BG84" s="27"/>
-      <c r="BH84" s="27"/>
-      <c r="BI84" s="27"/>
-      <c r="BJ84" s="26">
+      <c r="BG84" s="24"/>
+      <c r="BH84" s="24"/>
+      <c r="BI84" s="24"/>
+      <c r="BJ84" s="22">
         <v>2015</v>
       </c>
-      <c r="BK84" s="27"/>
-      <c r="BL84" s="27"/>
-      <c r="BM84" s="27"/>
-      <c r="BN84" s="26">
+      <c r="BK84" s="24"/>
+      <c r="BL84" s="24"/>
+      <c r="BM84" s="24"/>
+      <c r="BN84" s="22">
         <v>2016</v>
       </c>
-      <c r="BO84" s="27"/>
-      <c r="BP84" s="27"/>
-      <c r="BQ84" s="27"/>
-      <c r="BR84" s="26">
+      <c r="BO84" s="24"/>
+      <c r="BP84" s="24"/>
+      <c r="BQ84" s="24"/>
+      <c r="BR84" s="22">
         <v>2017</v>
       </c>
-      <c r="BS84" s="27"/>
-      <c r="BT84" s="27"/>
-      <c r="BU84" s="27"/>
-      <c r="BV84" s="29">
+      <c r="BS84" s="24"/>
+      <c r="BT84" s="24"/>
+      <c r="BU84" s="24"/>
+      <c r="BV84" s="22">
         <v>2018</v>
       </c>
-      <c r="BW84" s="30"/>
-      <c r="BX84" s="30"/>
-      <c r="BY84" s="30"/>
-      <c r="BZ84" s="26">
+      <c r="BW84" s="24"/>
+      <c r="BX84" s="24"/>
+      <c r="BY84" s="24"/>
+      <c r="BZ84" s="22">
         <v>2019</v>
       </c>
-      <c r="CA84" s="27"/>
-      <c r="CB84" s="27"/>
-      <c r="CC84" s="27"/>
-      <c r="CD84" s="26">
+      <c r="CA84" s="24"/>
+      <c r="CB84" s="24"/>
+      <c r="CC84" s="24"/>
+      <c r="CD84" s="22">
         <v>2020</v>
       </c>
-      <c r="CE84" s="26"/>
-      <c r="CF84" s="26"/>
-      <c r="CG84" s="26"/>
-      <c r="CH84" s="26">
+      <c r="CE84" s="24"/>
+      <c r="CF84" s="24"/>
+      <c r="CG84" s="24"/>
+      <c r="CH84" s="22">
         <v>2021</v>
       </c>
-      <c r="CI84" s="26"/>
-      <c r="CJ84" s="26"/>
-      <c r="CK84" s="26"/>
-      <c r="CL84" s="25">
+      <c r="CI84" s="22"/>
+      <c r="CJ84" s="22"/>
+      <c r="CK84" s="22"/>
+      <c r="CL84" s="22">
         <v>2022</v>
       </c>
+      <c r="CM84" s="22"/>
     </row>
-    <row r="85" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>4</v>
       </c>
@@ -32008,16 +31924,16 @@
       <c r="BU85" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="BV85" s="18" t="s">
+      <c r="BV85" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="BW85" s="18" t="s">
+      <c r="BW85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="BX85" s="18" t="s">
+      <c r="BX85" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="BY85" s="18" t="s">
+      <c r="BY85" s="6" t="s">
         <v>9</v>
       </c>
       <c r="BZ85" s="6" t="s">
@@ -32059,11 +31975,14 @@
       <c r="CL85" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="CM85" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="86" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
     </row>
-    <row r="87" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>11</v>
       </c>
@@ -32283,16 +32202,16 @@
       <c r="BU87" s="12">
         <v>95.817320896964517</v>
       </c>
-      <c r="BV87" s="24">
+      <c r="BV87" s="12">
         <v>98.533371913087507</v>
       </c>
-      <c r="BW87" s="24">
+      <c r="BW87" s="12">
         <v>99.664960991046243</v>
       </c>
-      <c r="BX87" s="24">
+      <c r="BX87" s="12">
         <v>99.679205723213911</v>
       </c>
-      <c r="BY87" s="24">
+      <c r="BY87" s="12">
         <v>102.09842429518893</v>
       </c>
       <c r="BZ87" s="12">
@@ -32334,7 +32253,9 @@
       <c r="CL87" s="12">
         <v>113.86947749514169</v>
       </c>
-      <c r="CM87" s="11"/>
+      <c r="CM87" s="12">
+        <v>114.21113977721637</v>
+      </c>
       <c r="CN87" s="11"/>
       <c r="CO87" s="11"/>
       <c r="CP87" s="11"/>
@@ -32396,7 +32317,7 @@
       <c r="ET87" s="11"/>
       <c r="EU87" s="11"/>
     </row>
-    <row r="88" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>12</v>
       </c>
@@ -32616,16 +32537,16 @@
       <c r="BU88" s="12">
         <v>97.358439390513311</v>
       </c>
-      <c r="BV88" s="24">
+      <c r="BV88" s="12">
         <v>98.108031307708814</v>
       </c>
-      <c r="BW88" s="24">
+      <c r="BW88" s="12">
         <v>99.618360181809209</v>
       </c>
-      <c r="BX88" s="24">
+      <c r="BX88" s="12">
         <v>101.18023488970312</v>
       </c>
-      <c r="BY88" s="24">
+      <c r="BY88" s="12">
         <v>101.09294002593954</v>
       </c>
       <c r="BZ88" s="12">
@@ -32667,7 +32588,9 @@
       <c r="CL88" s="12">
         <v>107.74936487010709</v>
       </c>
-      <c r="CM88" s="11"/>
+      <c r="CM88" s="12">
+        <v>108.43868958473841</v>
+      </c>
       <c r="CN88" s="11"/>
       <c r="CO88" s="11"/>
       <c r="CP88" s="11"/>
@@ -32729,7 +32652,7 @@
       <c r="ET88" s="11"/>
       <c r="EU88" s="11"/>
     </row>
-    <row r="89" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
@@ -32802,10 +32725,10 @@
       <c r="BS89" s="11"/>
       <c r="BT89" s="11"/>
       <c r="BU89" s="11"/>
-      <c r="BV89" s="20"/>
-      <c r="BW89" s="20"/>
-      <c r="BX89" s="20"/>
-      <c r="BY89" s="20"/>
+      <c r="BV89" s="11"/>
+      <c r="BW89" s="11"/>
+      <c r="BX89" s="11"/>
+      <c r="BY89" s="11"/>
       <c r="BZ89" s="11"/>
       <c r="CA89" s="11"/>
       <c r="CB89" s="11"/>
@@ -32881,7 +32804,7 @@
       <c r="ET89" s="11"/>
       <c r="EU89" s="11"/>
     </row>
-    <row r="90" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>13</v>
       </c>
@@ -33101,16 +33024,16 @@
       <c r="BU90" s="12">
         <v>96.526081390947851</v>
       </c>
-      <c r="BV90" s="24">
+      <c r="BV90" s="12">
         <v>98.33184786051406</v>
       </c>
-      <c r="BW90" s="24">
+      <c r="BW90" s="12">
         <v>99.644124245913162</v>
       </c>
-      <c r="BX90" s="24">
+      <c r="BX90" s="12">
         <v>100.32996743605747</v>
       </c>
-      <c r="BY90" s="24">
+      <c r="BY90" s="12">
         <v>101.63841017038584</v>
       </c>
       <c r="BZ90" s="12">
@@ -33150,9 +33073,11 @@
         <v>108.77008249664846</v>
       </c>
       <c r="CL90" s="12">
-        <v>110.67792104999528</v>
-      </c>
-      <c r="CM90" s="11"/>
+        <v>110.615986997851</v>
+      </c>
+      <c r="CM90" s="12">
+        <v>111.11098359397917</v>
+      </c>
       <c r="CN90" s="11"/>
       <c r="CO90" s="11"/>
       <c r="CP90" s="11"/>
@@ -33214,7 +33139,7 @@
       <c r="ET90" s="11"/>
       <c r="EU90" s="11"/>
     </row>
-    <row r="91" spans="1:151" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:151" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -33288,10 +33213,10 @@
       <c r="BS91" s="9"/>
       <c r="BT91" s="9"/>
       <c r="BU91" s="9"/>
-      <c r="BV91" s="22"/>
-      <c r="BW91" s="22"/>
-      <c r="BX91" s="22"/>
-      <c r="BY91" s="22"/>
+      <c r="BV91" s="9"/>
+      <c r="BW91" s="9"/>
+      <c r="BX91" s="9"/>
+      <c r="BY91" s="9"/>
       <c r="BZ91" s="9"/>
       <c r="CA91" s="9"/>
       <c r="CB91" s="9"/>
@@ -33305,181 +33230,183 @@
       <c r="CJ91" s="9"/>
       <c r="CK91" s="9"/>
       <c r="CL91" s="9"/>
+      <c r="CM91" s="9"/>
     </row>
-    <row r="92" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="101" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
-      <c r="B103" s="26">
+      <c r="B103" s="22">
         <v>2000</v>
       </c>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="26">
+      <c r="C103" s="24"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="22">
         <v>2001</v>
       </c>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="26">
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="22">
         <v>2002</v>
       </c>
-      <c r="K103" s="27"/>
-      <c r="L103" s="27"/>
-      <c r="M103" s="27"/>
-      <c r="N103" s="26">
+      <c r="K103" s="24"/>
+      <c r="L103" s="24"/>
+      <c r="M103" s="24"/>
+      <c r="N103" s="22">
         <v>2003</v>
       </c>
-      <c r="O103" s="27"/>
-      <c r="P103" s="27"/>
-      <c r="Q103" s="27"/>
-      <c r="R103" s="26">
+      <c r="O103" s="24"/>
+      <c r="P103" s="24"/>
+      <c r="Q103" s="24"/>
+      <c r="R103" s="22">
         <v>2004</v>
       </c>
-      <c r="S103" s="27"/>
-      <c r="T103" s="27"/>
-      <c r="U103" s="27"/>
-      <c r="V103" s="26">
+      <c r="S103" s="24"/>
+      <c r="T103" s="24"/>
+      <c r="U103" s="24"/>
+      <c r="V103" s="22">
         <v>2005</v>
       </c>
-      <c r="W103" s="27"/>
-      <c r="X103" s="27"/>
-      <c r="Y103" s="27"/>
-      <c r="Z103" s="26">
+      <c r="W103" s="24"/>
+      <c r="X103" s="24"/>
+      <c r="Y103" s="24"/>
+      <c r="Z103" s="22">
         <v>2006</v>
       </c>
-      <c r="AA103" s="27"/>
-      <c r="AB103" s="27"/>
-      <c r="AC103" s="27"/>
-      <c r="AD103" s="26">
+      <c r="AA103" s="24"/>
+      <c r="AB103" s="24"/>
+      <c r="AC103" s="24"/>
+      <c r="AD103" s="22">
         <v>2007</v>
       </c>
-      <c r="AE103" s="27"/>
-      <c r="AF103" s="27"/>
-      <c r="AG103" s="27"/>
-      <c r="AH103" s="26">
+      <c r="AE103" s="24"/>
+      <c r="AF103" s="24"/>
+      <c r="AG103" s="24"/>
+      <c r="AH103" s="22">
         <v>2008</v>
       </c>
-      <c r="AI103" s="27"/>
-      <c r="AJ103" s="27"/>
-      <c r="AK103" s="27"/>
-      <c r="AL103" s="26">
+      <c r="AI103" s="24"/>
+      <c r="AJ103" s="24"/>
+      <c r="AK103" s="24"/>
+      <c r="AL103" s="22">
         <v>2009</v>
       </c>
-      <c r="AM103" s="27"/>
-      <c r="AN103" s="27"/>
-      <c r="AO103" s="27"/>
-      <c r="AP103" s="26">
+      <c r="AM103" s="24"/>
+      <c r="AN103" s="24"/>
+      <c r="AO103" s="24"/>
+      <c r="AP103" s="22">
         <v>2010</v>
       </c>
-      <c r="AQ103" s="27"/>
-      <c r="AR103" s="27"/>
-      <c r="AS103" s="27"/>
-      <c r="AT103" s="26">
+      <c r="AQ103" s="24"/>
+      <c r="AR103" s="24"/>
+      <c r="AS103" s="24"/>
+      <c r="AT103" s="22">
         <v>2011</v>
       </c>
-      <c r="AU103" s="27"/>
-      <c r="AV103" s="27"/>
-      <c r="AW103" s="27"/>
-      <c r="AX103" s="26">
+      <c r="AU103" s="24"/>
+      <c r="AV103" s="24"/>
+      <c r="AW103" s="24"/>
+      <c r="AX103" s="22">
         <v>2012</v>
       </c>
-      <c r="AY103" s="27"/>
-      <c r="AZ103" s="27"/>
-      <c r="BA103" s="27"/>
-      <c r="BB103" s="26">
+      <c r="AY103" s="24"/>
+      <c r="AZ103" s="24"/>
+      <c r="BA103" s="24"/>
+      <c r="BB103" s="22">
         <v>2013</v>
       </c>
-      <c r="BC103" s="27"/>
-      <c r="BD103" s="27"/>
-      <c r="BE103" s="27"/>
-      <c r="BF103" s="26">
+      <c r="BC103" s="24"/>
+      <c r="BD103" s="24"/>
+      <c r="BE103" s="24"/>
+      <c r="BF103" s="22">
         <v>2014</v>
       </c>
-      <c r="BG103" s="27"/>
-      <c r="BH103" s="27"/>
-      <c r="BI103" s="27"/>
-      <c r="BJ103" s="26">
+      <c r="BG103" s="24"/>
+      <c r="BH103" s="24"/>
+      <c r="BI103" s="24"/>
+      <c r="BJ103" s="22">
         <v>2015</v>
       </c>
-      <c r="BK103" s="27"/>
-      <c r="BL103" s="27"/>
-      <c r="BM103" s="27"/>
-      <c r="BN103" s="26">
+      <c r="BK103" s="24"/>
+      <c r="BL103" s="24"/>
+      <c r="BM103" s="24"/>
+      <c r="BN103" s="22">
         <v>2016</v>
       </c>
-      <c r="BO103" s="27"/>
-      <c r="BP103" s="27"/>
-      <c r="BQ103" s="27"/>
-      <c r="BR103" s="26">
+      <c r="BO103" s="24"/>
+      <c r="BP103" s="24"/>
+      <c r="BQ103" s="24"/>
+      <c r="BR103" s="22">
         <v>2017</v>
       </c>
-      <c r="BS103" s="27"/>
-      <c r="BT103" s="27"/>
-      <c r="BU103" s="27"/>
-      <c r="BV103" s="29">
+      <c r="BS103" s="24"/>
+      <c r="BT103" s="24"/>
+      <c r="BU103" s="24"/>
+      <c r="BV103" s="22">
         <v>2018</v>
       </c>
-      <c r="BW103" s="30"/>
-      <c r="BX103" s="30"/>
-      <c r="BY103" s="30"/>
-      <c r="BZ103" s="26">
+      <c r="BW103" s="24"/>
+      <c r="BX103" s="24"/>
+      <c r="BY103" s="24"/>
+      <c r="BZ103" s="22">
         <v>2019</v>
       </c>
-      <c r="CA103" s="27"/>
-      <c r="CB103" s="27"/>
-      <c r="CC103" s="27"/>
-      <c r="CD103" s="26">
+      <c r="CA103" s="24"/>
+      <c r="CB103" s="24"/>
+      <c r="CC103" s="24"/>
+      <c r="CD103" s="22">
         <v>2020</v>
       </c>
-      <c r="CE103" s="26"/>
-      <c r="CF103" s="26"/>
-      <c r="CG103" s="26"/>
-      <c r="CH103" s="26">
+      <c r="CE103" s="24"/>
+      <c r="CF103" s="24"/>
+      <c r="CG103" s="24"/>
+      <c r="CH103" s="22">
         <v>2021</v>
       </c>
-      <c r="CI103" s="26"/>
-      <c r="CJ103" s="26"/>
-      <c r="CK103" s="26"/>
-      <c r="CL103" s="25">
+      <c r="CI103" s="22"/>
+      <c r="CJ103" s="22"/>
+      <c r="CK103" s="22"/>
+      <c r="CL103" s="22">
         <v>2022</v>
       </c>
+      <c r="CM103" s="22"/>
     </row>
-    <row r="104" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>4</v>
       </c>
@@ -33699,16 +33626,16 @@
       <c r="BU104" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="BV104" s="18" t="s">
+      <c r="BV104" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="BW104" s="18" t="s">
+      <c r="BW104" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="BX104" s="18" t="s">
+      <c r="BX104" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="BY104" s="18" t="s">
+      <c r="BY104" s="6" t="s">
         <v>9</v>
       </c>
       <c r="BZ104" s="6" t="s">
@@ -33750,11 +33677,14 @@
       <c r="CL104" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="CM104" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="105" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
     </row>
-    <row r="106" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>11</v>
       </c>
@@ -33974,16 +33904,16 @@
       <c r="BU106" s="12">
         <v>53.613415284160894</v>
       </c>
-      <c r="BV106" s="24">
+      <c r="BV106" s="12">
         <v>52.728388943525296</v>
       </c>
-      <c r="BW106" s="24">
+      <c r="BW106" s="12">
         <v>55.29829222129711</v>
       </c>
-      <c r="BX106" s="24">
+      <c r="BX106" s="12">
         <v>56.278215988133965</v>
       </c>
-      <c r="BY106" s="24">
+      <c r="BY106" s="12">
         <v>54.495028116848012</v>
       </c>
       <c r="BZ106" s="12">
@@ -34023,9 +33953,11 @@
         <v>48.059138135963934</v>
       </c>
       <c r="CL106" s="12">
-        <v>49.231206650876864</v>
-      </c>
-      <c r="CM106" s="11"/>
+        <v>48.217030867477916</v>
+      </c>
+      <c r="CM106" s="12">
+        <v>47.585596451846847</v>
+      </c>
       <c r="CN106" s="11"/>
       <c r="CO106" s="11"/>
       <c r="CP106" s="11"/>
@@ -34087,7 +34019,7 @@
       <c r="ET106" s="11"/>
       <c r="EU106" s="11"/>
     </row>
-    <row r="107" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>12</v>
       </c>
@@ -34307,16 +34239,16 @@
       <c r="BU107" s="12">
         <v>46.386584715839113</v>
       </c>
-      <c r="BV107" s="24">
+      <c r="BV107" s="12">
         <v>47.271611056474718</v>
       </c>
-      <c r="BW107" s="24">
+      <c r="BW107" s="12">
         <v>44.701707778702904</v>
       </c>
-      <c r="BX107" s="24">
+      <c r="BX107" s="12">
         <v>43.721784011866028</v>
       </c>
-      <c r="BY107" s="24">
+      <c r="BY107" s="12">
         <v>45.504971883152002</v>
       </c>
       <c r="BZ107" s="12">
@@ -34356,9 +34288,11 @@
         <v>51.940861864036059</v>
       </c>
       <c r="CL107" s="12">
-        <v>50.768793349123129</v>
-      </c>
-      <c r="CM107" s="11"/>
+        <v>51.782969132522069</v>
+      </c>
+      <c r="CM107" s="12">
+        <v>52.414403548153153</v>
+      </c>
       <c r="CN107" s="11"/>
       <c r="CO107" s="11"/>
       <c r="CP107" s="11"/>
@@ -34420,7 +34354,7 @@
       <c r="ET107" s="11"/>
       <c r="EU107" s="11"/>
     </row>
-    <row r="108" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -34493,10 +34427,10 @@
       <c r="BS108" s="11"/>
       <c r="BT108" s="11"/>
       <c r="BU108" s="11"/>
-      <c r="BV108" s="20"/>
-      <c r="BW108" s="20"/>
-      <c r="BX108" s="20"/>
-      <c r="BY108" s="20"/>
+      <c r="BV108" s="11"/>
+      <c r="BW108" s="11"/>
+      <c r="BX108" s="11"/>
+      <c r="BY108" s="11"/>
       <c r="BZ108" s="11"/>
       <c r="CA108" s="11"/>
       <c r="CB108" s="11"/>
@@ -34572,7 +34506,7 @@
       <c r="ET108" s="11"/>
       <c r="EU108" s="11"/>
     </row>
-    <row r="109" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>13</v>
       </c>
@@ -34792,16 +34726,16 @@
       <c r="BU109" s="12">
         <v>100</v>
       </c>
-      <c r="BV109" s="24">
+      <c r="BV109" s="12">
         <v>100</v>
       </c>
-      <c r="BW109" s="24">
+      <c r="BW109" s="12">
         <v>100</v>
       </c>
-      <c r="BX109" s="24">
+      <c r="BX109" s="12">
         <v>100</v>
       </c>
-      <c r="BY109" s="24">
+      <c r="BY109" s="12">
         <v>100</v>
       </c>
       <c r="BZ109" s="12">
@@ -34843,7 +34777,9 @@
       <c r="CL109" s="12">
         <v>100</v>
       </c>
-      <c r="CM109" s="11"/>
+      <c r="CM109" s="12">
+        <v>100</v>
+      </c>
       <c r="CN109" s="11"/>
       <c r="CO109" s="11"/>
       <c r="CP109" s="11"/>
@@ -34905,7 +34841,7 @@
       <c r="ET109" s="11"/>
       <c r="EU109" s="11"/>
     </row>
-    <row r="110" spans="1:151" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:151" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="9"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
@@ -34979,10 +34915,10 @@
       <c r="BS110" s="9"/>
       <c r="BT110" s="9"/>
       <c r="BU110" s="9"/>
-      <c r="BV110" s="22"/>
-      <c r="BW110" s="22"/>
-      <c r="BX110" s="22"/>
-      <c r="BY110" s="22"/>
+      <c r="BV110" s="9"/>
+      <c r="BW110" s="9"/>
+      <c r="BX110" s="9"/>
+      <c r="BY110" s="9"/>
       <c r="BZ110" s="9"/>
       <c r="CA110" s="9"/>
       <c r="CB110" s="9"/>
@@ -34996,13 +34932,14 @@
       <c r="CJ110" s="9"/>
       <c r="CK110" s="9"/>
       <c r="CL110" s="9"/>
+      <c r="CM110" s="9"/>
     </row>
-    <row r="111" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
@@ -35075,10 +35012,10 @@
       <c r="BS112" s="11"/>
       <c r="BT112" s="11"/>
       <c r="BU112" s="11"/>
-      <c r="BV112" s="20"/>
-      <c r="BW112" s="20"/>
-      <c r="BX112" s="20"/>
-      <c r="BY112" s="20"/>
+      <c r="BV112" s="11"/>
+      <c r="BW112" s="11"/>
+      <c r="BX112" s="11"/>
+      <c r="BY112" s="11"/>
       <c r="BZ112" s="11"/>
       <c r="CA112" s="11"/>
       <c r="CB112" s="11"/>
@@ -35154,7 +35091,7 @@
       <c r="ET112" s="11"/>
       <c r="EU112" s="11"/>
     </row>
-    <row r="113" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
@@ -35227,10 +35164,10 @@
       <c r="BS113" s="11"/>
       <c r="BT113" s="11"/>
       <c r="BU113" s="11"/>
-      <c r="BV113" s="20"/>
-      <c r="BW113" s="20"/>
-      <c r="BX113" s="20"/>
-      <c r="BY113" s="20"/>
+      <c r="BV113" s="11"/>
+      <c r="BW113" s="11"/>
+      <c r="BX113" s="11"/>
+      <c r="BY113" s="11"/>
       <c r="BZ113" s="11"/>
       <c r="CA113" s="11"/>
       <c r="CB113" s="11"/>
@@ -35306,175 +35243,176 @@
       <c r="ET113" s="11"/>
       <c r="EU113" s="11"/>
     </row>
-    <row r="114" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="120" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
-      <c r="B122" s="26">
+      <c r="B122" s="22">
         <v>2000</v>
       </c>
-      <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="26">
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="22">
         <v>2001</v>
       </c>
-      <c r="G122" s="27"/>
-      <c r="H122" s="27"/>
-      <c r="I122" s="27"/>
-      <c r="J122" s="26">
+      <c r="G122" s="24"/>
+      <c r="H122" s="24"/>
+      <c r="I122" s="24"/>
+      <c r="J122" s="22">
         <v>2002</v>
       </c>
-      <c r="K122" s="27"/>
-      <c r="L122" s="27"/>
-      <c r="M122" s="27"/>
-      <c r="N122" s="26">
+      <c r="K122" s="24"/>
+      <c r="L122" s="24"/>
+      <c r="M122" s="24"/>
+      <c r="N122" s="22">
         <v>2003</v>
       </c>
-      <c r="O122" s="27"/>
-      <c r="P122" s="27"/>
-      <c r="Q122" s="27"/>
-      <c r="R122" s="26">
+      <c r="O122" s="24"/>
+      <c r="P122" s="24"/>
+      <c r="Q122" s="24"/>
+      <c r="R122" s="22">
         <v>2004</v>
       </c>
-      <c r="S122" s="27"/>
-      <c r="T122" s="27"/>
-      <c r="U122" s="27"/>
-      <c r="V122" s="26">
+      <c r="S122" s="24"/>
+      <c r="T122" s="24"/>
+      <c r="U122" s="24"/>
+      <c r="V122" s="22">
         <v>2005</v>
       </c>
-      <c r="W122" s="27"/>
-      <c r="X122" s="27"/>
-      <c r="Y122" s="27"/>
-      <c r="Z122" s="26">
+      <c r="W122" s="24"/>
+      <c r="X122" s="24"/>
+      <c r="Y122" s="24"/>
+      <c r="Z122" s="22">
         <v>2006</v>
       </c>
-      <c r="AA122" s="27"/>
-      <c r="AB122" s="27"/>
-      <c r="AC122" s="27"/>
-      <c r="AD122" s="26">
+      <c r="AA122" s="24"/>
+      <c r="AB122" s="24"/>
+      <c r="AC122" s="24"/>
+      <c r="AD122" s="22">
         <v>2007</v>
       </c>
-      <c r="AE122" s="27"/>
-      <c r="AF122" s="27"/>
-      <c r="AG122" s="27"/>
-      <c r="AH122" s="26">
+      <c r="AE122" s="24"/>
+      <c r="AF122" s="24"/>
+      <c r="AG122" s="24"/>
+      <c r="AH122" s="22">
         <v>2008</v>
       </c>
-      <c r="AI122" s="27"/>
-      <c r="AJ122" s="27"/>
-      <c r="AK122" s="27"/>
-      <c r="AL122" s="26">
+      <c r="AI122" s="24"/>
+      <c r="AJ122" s="24"/>
+      <c r="AK122" s="24"/>
+      <c r="AL122" s="22">
         <v>2009</v>
       </c>
-      <c r="AM122" s="27"/>
-      <c r="AN122" s="27"/>
-      <c r="AO122" s="27"/>
-      <c r="AP122" s="26">
+      <c r="AM122" s="24"/>
+      <c r="AN122" s="24"/>
+      <c r="AO122" s="24"/>
+      <c r="AP122" s="22">
         <v>2010</v>
       </c>
-      <c r="AQ122" s="27"/>
-      <c r="AR122" s="27"/>
-      <c r="AS122" s="27"/>
-      <c r="AT122" s="26">
+      <c r="AQ122" s="24"/>
+      <c r="AR122" s="24"/>
+      <c r="AS122" s="24"/>
+      <c r="AT122" s="22">
         <v>2011</v>
       </c>
-      <c r="AU122" s="27"/>
-      <c r="AV122" s="27"/>
-      <c r="AW122" s="27"/>
-      <c r="AX122" s="26">
+      <c r="AU122" s="24"/>
+      <c r="AV122" s="24"/>
+      <c r="AW122" s="24"/>
+      <c r="AX122" s="22">
         <v>2012</v>
       </c>
-      <c r="AY122" s="27"/>
-      <c r="AZ122" s="27"/>
-      <c r="BA122" s="27"/>
-      <c r="BB122" s="26">
+      <c r="AY122" s="24"/>
+      <c r="AZ122" s="24"/>
+      <c r="BA122" s="24"/>
+      <c r="BB122" s="22">
         <v>2013</v>
       </c>
-      <c r="BC122" s="27"/>
-      <c r="BD122" s="27"/>
-      <c r="BE122" s="27"/>
-      <c r="BF122" s="26">
+      <c r="BC122" s="24"/>
+      <c r="BD122" s="24"/>
+      <c r="BE122" s="24"/>
+      <c r="BF122" s="22">
         <v>2014</v>
       </c>
-      <c r="BG122" s="27"/>
-      <c r="BH122" s="27"/>
-      <c r="BI122" s="27"/>
-      <c r="BJ122" s="26">
+      <c r="BG122" s="24"/>
+      <c r="BH122" s="24"/>
+      <c r="BI122" s="24"/>
+      <c r="BJ122" s="22">
         <v>2015</v>
       </c>
-      <c r="BK122" s="27"/>
-      <c r="BL122" s="27"/>
-      <c r="BM122" s="27"/>
-      <c r="BN122" s="26">
+      <c r="BK122" s="24"/>
+      <c r="BL122" s="24"/>
+      <c r="BM122" s="24"/>
+      <c r="BN122" s="22">
         <v>2016</v>
       </c>
-      <c r="BO122" s="27"/>
-      <c r="BP122" s="27"/>
-      <c r="BQ122" s="27"/>
-      <c r="BR122" s="26">
+      <c r="BO122" s="24"/>
+      <c r="BP122" s="24"/>
+      <c r="BQ122" s="24"/>
+      <c r="BR122" s="22">
         <v>2017</v>
       </c>
-      <c r="BS122" s="27"/>
-      <c r="BT122" s="27"/>
-      <c r="BU122" s="27"/>
-      <c r="BV122" s="29">
+      <c r="BS122" s="24"/>
+      <c r="BT122" s="24"/>
+      <c r="BU122" s="24"/>
+      <c r="BV122" s="22">
         <v>2018</v>
       </c>
-      <c r="BW122" s="30"/>
-      <c r="BX122" s="30"/>
-      <c r="BY122" s="30"/>
-      <c r="BZ122" s="26">
+      <c r="BW122" s="24"/>
+      <c r="BX122" s="24"/>
+      <c r="BY122" s="24"/>
+      <c r="BZ122" s="22">
         <v>2019</v>
       </c>
-      <c r="CA122" s="27"/>
-      <c r="CB122" s="27"/>
-      <c r="CC122" s="27"/>
-      <c r="CD122" s="26">
+      <c r="CA122" s="24"/>
+      <c r="CB122" s="24"/>
+      <c r="CC122" s="24"/>
+      <c r="CD122" s="22">
         <v>2020</v>
       </c>
-      <c r="CE122" s="26"/>
-      <c r="CF122" s="26"/>
-      <c r="CG122" s="26"/>
-      <c r="CH122" s="26">
+      <c r="CE122" s="24"/>
+      <c r="CF122" s="24"/>
+      <c r="CG122" s="24"/>
+      <c r="CH122" s="22">
         <v>2021</v>
       </c>
-      <c r="CI122" s="26"/>
-      <c r="CJ122" s="26"/>
-      <c r="CK122" s="26"/>
-      <c r="CL122" s="25">
+      <c r="CI122" s="22"/>
+      <c r="CJ122" s="22"/>
+      <c r="CK122" s="22"/>
+      <c r="CL122" s="22">
         <v>2022</v>
       </c>
+      <c r="CM122" s="22"/>
     </row>
-    <row r="123" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>4</v>
       </c>
@@ -35694,16 +35632,16 @@
       <c r="BU123" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="BV123" s="18" t="s">
+      <c r="BV123" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="BW123" s="18" t="s">
+      <c r="BW123" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="BX123" s="18" t="s">
+      <c r="BX123" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="BY123" s="18" t="s">
+      <c r="BY123" s="6" t="s">
         <v>9</v>
       </c>
       <c r="BZ123" s="6" t="s">
@@ -35745,11 +35683,14 @@
       <c r="CL123" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="CM123" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="124" spans="1:151" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:151" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
     </row>
-    <row r="125" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>11</v>
       </c>
@@ -35969,16 +35910,16 @@
       <c r="BU125" s="12">
         <v>54.009993589056279</v>
       </c>
-      <c r="BV125" s="24">
+      <c r="BV125" s="12">
         <v>52.620546915801512</v>
       </c>
-      <c r="BW125" s="24">
+      <c r="BW125" s="12">
         <v>55.286731122894494</v>
       </c>
-      <c r="BX125" s="24">
+      <c r="BX125" s="12">
         <v>56.645631719093068</v>
       </c>
-      <c r="BY125" s="24">
+      <c r="BY125" s="12">
         <v>54.249495604095287</v>
       </c>
       <c r="BZ125" s="12">
@@ -36018,9 +35959,11 @@
         <v>47.49738539006951</v>
       </c>
       <c r="CL125" s="12">
-        <v>47.851344563640673</v>
-      </c>
-      <c r="CM125" s="11"/>
+        <v>46.839368870727256</v>
+      </c>
+      <c r="CM125" s="12">
+        <v>46.293929269810278</v>
+      </c>
       <c r="CN125" s="11"/>
       <c r="CO125" s="11"/>
       <c r="CP125" s="11"/>
@@ -36082,7 +36025,7 @@
       <c r="ET125" s="11"/>
       <c r="EU125" s="11"/>
     </row>
-    <row r="126" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>12</v>
       </c>
@@ -36302,16 +36245,16 @@
       <c r="BU126" s="12">
         <v>45.990006410943728</v>
       </c>
-      <c r="BV126" s="24">
+      <c r="BV126" s="12">
         <v>47.379453084198488</v>
       </c>
-      <c r="BW126" s="24">
+      <c r="BW126" s="12">
         <v>44.713268877105492</v>
       </c>
-      <c r="BX126" s="24">
+      <c r="BX126" s="12">
         <v>43.354368280906918</v>
       </c>
-      <c r="BY126" s="24">
+      <c r="BY126" s="12">
         <v>45.750504395904713</v>
       </c>
       <c r="BZ126" s="12">
@@ -36351,9 +36294,11 @@
         <v>52.502614609930497</v>
       </c>
       <c r="CL126" s="12">
-        <v>52.148655436359327</v>
-      </c>
-      <c r="CM126" s="11"/>
+        <v>53.160631129272737</v>
+      </c>
+      <c r="CM126" s="12">
+        <v>53.706070730189722</v>
+      </c>
       <c r="CN126" s="11"/>
       <c r="CO126" s="11"/>
       <c r="CP126" s="11"/>
@@ -36415,7 +36360,7 @@
       <c r="ET126" s="11"/>
       <c r="EU126" s="11"/>
     </row>
-    <row r="127" spans="1:151" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:151" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="11"/>
       <c r="C127" s="11"/>
       <c r="D127" s="11"/>
@@ -36488,10 +36433,10 @@
       <c r="BS127" s="11"/>
       <c r="BT127" s="11"/>
       <c r="BU127" s="11"/>
-      <c r="BV127" s="20"/>
-      <c r="BW127" s="20"/>
-      <c r="BX127" s="20"/>
-      <c r="BY127" s="20"/>
+      <c r="BV127" s="11"/>
+      <c r="BW127" s="11"/>
+      <c r="BX127" s="11"/>
+      <c r="BY127" s="11"/>
       <c r="BZ127" s="11"/>
       <c r="CA127" s="11"/>
       <c r="CB127" s="11"/>
@@ -36567,7 +36512,7 @@
       <c r="ET127" s="11"/>
       <c r="EU127" s="11"/>
     </row>
-    <row r="128" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:151" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
         <v>13</v>
       </c>
@@ -36787,16 +36732,16 @@
       <c r="BU128" s="12">
         <v>100</v>
       </c>
-      <c r="BV128" s="24">
+      <c r="BV128" s="12">
         <v>100</v>
       </c>
-      <c r="BW128" s="24">
+      <c r="BW128" s="12">
         <v>100</v>
       </c>
-      <c r="BX128" s="24">
+      <c r="BX128" s="12">
         <v>100</v>
       </c>
-      <c r="BY128" s="24">
+      <c r="BY128" s="12">
         <v>100</v>
       </c>
       <c r="BZ128" s="12">
@@ -36838,7 +36783,9 @@
       <c r="CL128" s="12">
         <v>100</v>
       </c>
-      <c r="CM128" s="11"/>
+      <c r="CM128" s="12">
+        <v>100</v>
+      </c>
       <c r="CN128" s="11"/>
       <c r="CO128" s="11"/>
       <c r="CP128" s="11"/>
@@ -36900,7 +36847,7 @@
       <c r="ET128" s="11"/>
       <c r="EU128" s="11"/>
     </row>
-    <row r="129" spans="1:151" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:151" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="9"/>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -36974,10 +36921,10 @@
       <c r="BS129" s="9"/>
       <c r="BT129" s="9"/>
       <c r="BU129" s="9"/>
-      <c r="BV129" s="22"/>
-      <c r="BW129" s="22"/>
-      <c r="BX129" s="22"/>
-      <c r="BY129" s="22"/>
+      <c r="BV129" s="9"/>
+      <c r="BW129" s="9"/>
+      <c r="BX129" s="9"/>
+      <c r="BY129" s="9"/>
       <c r="BZ129" s="9"/>
       <c r="CA129" s="9"/>
       <c r="CB129" s="9"/>
@@ -36991,13 +36938,14 @@
       <c r="CJ129" s="9"/>
       <c r="CK129" s="9"/>
       <c r="CL129" s="9"/>
+      <c r="CM129" s="9"/>
     </row>
-    <row r="130" spans="1:151" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:151" s="14" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:151" s="14" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="13"/>
       <c r="C131" s="13"/>
@@ -37071,24 +37019,24 @@
       <c r="BS131" s="13"/>
       <c r="BT131" s="13"/>
       <c r="BU131" s="13"/>
-      <c r="BV131" s="17"/>
-      <c r="BW131" s="17"/>
-      <c r="BX131" s="17"/>
-      <c r="BY131" s="17"/>
+      <c r="BV131" s="3"/>
+      <c r="BW131" s="3"/>
+      <c r="BX131" s="3"/>
+      <c r="BY131" s="3"/>
       <c r="BZ131" s="3"/>
       <c r="CA131" s="3"/>
       <c r="CB131" s="3"/>
       <c r="CC131" s="3"/>
-      <c r="CD131" s="13"/>
-      <c r="CE131" s="13"/>
-      <c r="CF131" s="13"/>
-      <c r="CG131" s="13"/>
-      <c r="CH131" s="13"/>
-      <c r="CI131" s="13"/>
-      <c r="CJ131" s="13"/>
-      <c r="CK131" s="13"/>
-      <c r="CL131" s="13"/>
-      <c r="CM131" s="13"/>
+      <c r="CD131" s="3"/>
+      <c r="CE131" s="3"/>
+      <c r="CF131" s="3"/>
+      <c r="CG131" s="3"/>
+      <c r="CH131" s="3"/>
+      <c r="CI131" s="3"/>
+      <c r="CJ131" s="3"/>
+      <c r="CK131" s="3"/>
+      <c r="CL131" s="3"/>
+      <c r="CM131" s="3"/>
       <c r="CN131" s="13"/>
       <c r="CO131" s="13"/>
       <c r="CP131" s="13"/>
@@ -37150,7 +37098,7 @@
       <c r="ET131" s="13"/>
       <c r="EU131" s="13"/>
     </row>
-    <row r="132" spans="1:151" s="14" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:151" s="14" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="13"/>
       <c r="C132" s="13"/>
@@ -37224,24 +37172,24 @@
       <c r="BS132" s="13"/>
       <c r="BT132" s="13"/>
       <c r="BU132" s="13"/>
-      <c r="BV132" s="17"/>
-      <c r="BW132" s="17"/>
-      <c r="BX132" s="17"/>
-      <c r="BY132" s="17"/>
+      <c r="BV132" s="3"/>
+      <c r="BW132" s="3"/>
+      <c r="BX132" s="3"/>
+      <c r="BY132" s="3"/>
       <c r="BZ132" s="3"/>
       <c r="CA132" s="3"/>
       <c r="CB132" s="3"/>
       <c r="CC132" s="3"/>
-      <c r="CD132" s="13"/>
-      <c r="CE132" s="13"/>
-      <c r="CF132" s="13"/>
-      <c r="CG132" s="13"/>
-      <c r="CH132" s="13"/>
-      <c r="CI132" s="13"/>
-      <c r="CJ132" s="13"/>
-      <c r="CK132" s="13"/>
-      <c r="CL132" s="13"/>
-      <c r="CM132" s="13"/>
+      <c r="CD132" s="3"/>
+      <c r="CE132" s="3"/>
+      <c r="CF132" s="3"/>
+      <c r="CG132" s="3"/>
+      <c r="CH132" s="3"/>
+      <c r="CI132" s="3"/>
+      <c r="CJ132" s="3"/>
+      <c r="CK132" s="3"/>
+      <c r="CL132" s="3"/>
+      <c r="CM132" s="3"/>
       <c r="CN132" s="13"/>
       <c r="CO132" s="13"/>
       <c r="CP132" s="13"/>
@@ -37304,7 +37252,7 @@
       <c r="EU132" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="152">
+  <mergeCells count="159">
     <mergeCell ref="BZ28:CC28"/>
     <mergeCell ref="BV47:BY47"/>
     <mergeCell ref="BR47:BU47"/>
@@ -37329,12 +37277,6 @@
     <mergeCell ref="BV28:BY28"/>
     <mergeCell ref="BR66:BU66"/>
     <mergeCell ref="BV66:BY66"/>
-    <mergeCell ref="BJ66:BM66"/>
-    <mergeCell ref="BN66:BQ66"/>
-    <mergeCell ref="AL66:AO66"/>
-    <mergeCell ref="AP66:AS66"/>
-    <mergeCell ref="V47:Y47"/>
-    <mergeCell ref="AL28:AO28"/>
     <mergeCell ref="AP28:AS28"/>
     <mergeCell ref="AT28:AW28"/>
     <mergeCell ref="AX28:BA28"/>
@@ -37345,8 +37287,23 @@
     <mergeCell ref="AP47:AS47"/>
     <mergeCell ref="AT47:AW47"/>
     <mergeCell ref="AX47:BA47"/>
-    <mergeCell ref="AX66:BA66"/>
-    <mergeCell ref="AT66:AW66"/>
+    <mergeCell ref="BB47:BE47"/>
+    <mergeCell ref="BF47:BI47"/>
+    <mergeCell ref="BJ47:BM47"/>
+    <mergeCell ref="BN47:BQ47"/>
+    <mergeCell ref="BR9:BU9"/>
+    <mergeCell ref="BV9:BY9"/>
+    <mergeCell ref="BJ9:BM9"/>
+    <mergeCell ref="BN9:BQ9"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="R28:U28"/>
+    <mergeCell ref="V28:Y28"/>
+    <mergeCell ref="Z28:AC28"/>
+    <mergeCell ref="AD28:AG28"/>
+    <mergeCell ref="AH28:AK28"/>
     <mergeCell ref="V9:Y9"/>
     <mergeCell ref="Z9:AC9"/>
     <mergeCell ref="AD9:AG9"/>
@@ -37358,15 +37315,6 @@
     <mergeCell ref="AT9:AW9"/>
     <mergeCell ref="AX9:BA9"/>
     <mergeCell ref="BB9:BE9"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="R28:U28"/>
-    <mergeCell ref="V28:Y28"/>
-    <mergeCell ref="Z28:AC28"/>
-    <mergeCell ref="AD28:AG28"/>
-    <mergeCell ref="AH28:AK28"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="N9:Q9"/>
@@ -37387,10 +37335,10 @@
     <mergeCell ref="BF66:BI66"/>
     <mergeCell ref="N66:Q66"/>
     <mergeCell ref="R66:U66"/>
-    <mergeCell ref="V66:Y66"/>
-    <mergeCell ref="Z66:AC66"/>
-    <mergeCell ref="AD66:AG66"/>
-    <mergeCell ref="AH66:AK66"/>
+    <mergeCell ref="AL66:AO66"/>
+    <mergeCell ref="AP66:AS66"/>
+    <mergeCell ref="V47:Y47"/>
+    <mergeCell ref="AL28:AO28"/>
     <mergeCell ref="B103:E103"/>
     <mergeCell ref="F103:I103"/>
     <mergeCell ref="J103:M103"/>
@@ -37404,16 +37352,8 @@
     <mergeCell ref="F84:I84"/>
     <mergeCell ref="J84:M84"/>
     <mergeCell ref="N84:Q84"/>
-    <mergeCell ref="AL84:AO84"/>
-    <mergeCell ref="AP84:AS84"/>
-    <mergeCell ref="AT84:AW84"/>
-    <mergeCell ref="AX84:BA84"/>
-    <mergeCell ref="AH84:AK84"/>
     <mergeCell ref="R103:U103"/>
     <mergeCell ref="V103:Y103"/>
-    <mergeCell ref="V84:Y84"/>
-    <mergeCell ref="Z84:AC84"/>
-    <mergeCell ref="AD84:AG84"/>
     <mergeCell ref="B122:E122"/>
     <mergeCell ref="F122:I122"/>
     <mergeCell ref="J122:M122"/>
@@ -37423,49 +37363,64 @@
     <mergeCell ref="Z122:AC122"/>
     <mergeCell ref="AD122:AG122"/>
     <mergeCell ref="AH122:AK122"/>
+    <mergeCell ref="V84:Y84"/>
+    <mergeCell ref="Z84:AC84"/>
+    <mergeCell ref="AD84:AG84"/>
+    <mergeCell ref="AH84:AK84"/>
+    <mergeCell ref="BF84:BI84"/>
+    <mergeCell ref="BB84:BE84"/>
+    <mergeCell ref="BJ66:BM66"/>
+    <mergeCell ref="BN66:BQ66"/>
+    <mergeCell ref="BF122:BI122"/>
+    <mergeCell ref="BJ122:BM122"/>
+    <mergeCell ref="BN122:BQ122"/>
+    <mergeCell ref="BJ103:BM103"/>
+    <mergeCell ref="BN103:BQ103"/>
     <mergeCell ref="AL122:AO122"/>
     <mergeCell ref="AP122:AS122"/>
     <mergeCell ref="AT122:AW122"/>
     <mergeCell ref="AX122:BA122"/>
     <mergeCell ref="BB122:BE122"/>
     <mergeCell ref="BF103:BI103"/>
-    <mergeCell ref="AL103:AO103"/>
-    <mergeCell ref="AP103:AS103"/>
-    <mergeCell ref="AT103:AW103"/>
-    <mergeCell ref="AX103:BA103"/>
-    <mergeCell ref="BF84:BI84"/>
-    <mergeCell ref="BB84:BE84"/>
-    <mergeCell ref="CH9:CK9"/>
-    <mergeCell ref="CH28:CK28"/>
+    <mergeCell ref="V66:Y66"/>
+    <mergeCell ref="Z66:AC66"/>
+    <mergeCell ref="AD66:AG66"/>
+    <mergeCell ref="AH66:AK66"/>
+    <mergeCell ref="AX66:BA66"/>
     <mergeCell ref="CD47:CG47"/>
     <mergeCell ref="CD66:CG66"/>
     <mergeCell ref="CH84:CK84"/>
     <mergeCell ref="CH103:CK103"/>
     <mergeCell ref="CH122:CK122"/>
-    <mergeCell ref="BB47:BE47"/>
-    <mergeCell ref="BF47:BI47"/>
-    <mergeCell ref="BJ47:BM47"/>
-    <mergeCell ref="BN47:BQ47"/>
     <mergeCell ref="BN84:BQ84"/>
+    <mergeCell ref="AL103:AO103"/>
+    <mergeCell ref="AP103:AS103"/>
+    <mergeCell ref="AT103:AW103"/>
+    <mergeCell ref="AX103:BA103"/>
+    <mergeCell ref="AT66:AW66"/>
     <mergeCell ref="BJ84:BM84"/>
-    <mergeCell ref="BF122:BI122"/>
-    <mergeCell ref="BJ122:BM122"/>
-    <mergeCell ref="BN122:BQ122"/>
-    <mergeCell ref="BJ103:BM103"/>
-    <mergeCell ref="BN103:BQ103"/>
-    <mergeCell ref="BR9:BU9"/>
-    <mergeCell ref="BV9:BY9"/>
-    <mergeCell ref="BJ9:BM9"/>
-    <mergeCell ref="BN9:BQ9"/>
+    <mergeCell ref="AL84:AO84"/>
+    <mergeCell ref="AP84:AS84"/>
+    <mergeCell ref="AT84:AW84"/>
+    <mergeCell ref="AX84:BA84"/>
+    <mergeCell ref="CL9:CM9"/>
+    <mergeCell ref="CL28:CM28"/>
+    <mergeCell ref="CH47:CI47"/>
+    <mergeCell ref="CH66:CI66"/>
+    <mergeCell ref="CL84:CM84"/>
+    <mergeCell ref="CL103:CM103"/>
+    <mergeCell ref="CL122:CM122"/>
+    <mergeCell ref="CH9:CK9"/>
+    <mergeCell ref="CH28:CK28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.3" top="1" bottom="0.16700000000000001" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="38" max="91" man="1"/>
-    <brk id="76" max="91" man="1"/>
-    <brk id="94" max="91" man="1"/>
+    <brk id="38" max="90" man="1"/>
+    <brk id="76" max="90" man="1"/>
+    <brk id="94" max="90" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>